<commit_message>
Consultado status profissional e leads
</commit_message>
<xml_diff>
--- a/Exercicios/Projeto02_Perfil_Dos_Clientes.xlsx
+++ b/Exercicios/Projeto02_Perfil_Dos_Clientes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10713"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\05-SQL\07-Projeto 2 - Perfil dos leads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guilhermefogolin/Projetos/Estudos-SQL/Exercicios/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2D4F773-FB4A-4985-B230-664058C08BB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB41DF81-AD16-754C-80E0-D6859B85B712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="6" r:id="rId1"/>
@@ -41,12 +41,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t>visitas (#)</t>
-  </si>
-  <si>
-    <t>gênero</t>
   </si>
   <si>
     <t>status profissional</t>
@@ -94,9 +91,6 @@
     <t>7-Veículos mais visitados por marca</t>
   </si>
   <si>
-    <t>leads (#)</t>
-  </si>
-  <si>
     <t>leads (%)</t>
   </si>
   <si>
@@ -104,6 +98,18 @@
   </si>
   <si>
     <t>veículos visitados (%)</t>
+  </si>
+  <si>
+    <t>Mulheres</t>
+  </si>
+  <si>
+    <t>Homens</t>
+  </si>
+  <si>
+    <t>Gênero</t>
+  </si>
+  <si>
+    <t>Leads (#)</t>
   </si>
 </sst>
 </file>
@@ -151,7 +157,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -161,6 +167,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -178,32 +190,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="17" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Porcentagem" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -232,7 +253,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="pt-BR"/>
   <c:roundedCorners val="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -312,7 +333,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>leads (#)</c:v>
+                  <c:v>Leads (#)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -418,13 +439,18 @@
             </c:extLst>
           </c:dLbls>
           <c:cat>
-            <c:numRef>
+            <c:strRef>
               <c:f>Output!$B$4:$B$5</c:f>
-              <c:numCache>
-                <c:formatCode>[$-416]mmm\-yy;@</c:formatCode>
+              <c:strCache>
                 <c:ptCount val="2"/>
-              </c:numCache>
-            </c:numRef>
+                <c:pt idx="0">
+                  <c:v>Mulheres</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Homens</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -432,6 +458,12 @@
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>15106</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10003</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -494,6 +526,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -501,7 +534,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -541,7 +573,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="pt-BR"/>
   <c:roundedCorners val="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -852,6 +884,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -859,7 +892,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -899,7 +931,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="pt-BR"/>
   <c:roundedCorners val="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1214,6 +1246,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1221,7 +1254,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1261,7 +1293,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="pt-BR"/>
   <c:roundedCorners val="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1593,7 +1625,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="pt-BR"/>
   <c:roundedCorners val="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1860,6 +1892,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1867,7 +1900,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1907,7 +1939,7 @@
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="pt-BR"/>
   <c:roundedCorners val="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -5400,8 +5432,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="9502912" y="190500"/>
-              <a:ext cx="5816628" cy="5592535"/>
+              <a:off x="10490337" y="190500"/>
+              <a:ext cx="6388128" cy="5592535"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -5420,9 +5452,9 @@
             <a:lstStyle/>
             <a:p>
               <a:r>
-                <a:rPr lang="en-US" sz="1100"/>
-                <a:t>This chart isn't available in your version of Excel.
-Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+                <a:rPr lang="pt-BR" sz="1100"/>
+                <a:t>Este gráfico não está disponível na sua versão de Excel.
+Editar esta forma ou salvar esta pasta de trabalho em um formato de arquivo diferente quebrará o gráfico permanentemente.</a:t>
               </a:r>
             </a:p>
           </xdr:txBody>
@@ -5522,6 +5554,157 @@
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
             <a:t>-- Colunas: gênero, leads(#)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" b="1">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>SELECT</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>	CASE</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>	WHEN i.gender = 'male' THEN 'Homens'</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>	WHEN i.gender = 'female' THEN 'Mulheres'</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>	END AS "Gênero",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>	COUNT(*) AS "Leads (#)"	</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>FROM sales.customers c</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>LEFT JOIN temp_tables.ibge_genders i</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>ON LOWER(c.first_name) = LOWER(i.first_name)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>GROUP BY i.gender;</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -6486,13 +6669,13 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" customWidth="1"/>
+    <col min="1" max="1" width="3.33203125" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6507,112 +6690,116 @@
   </sheetPr>
   <dimension ref="B2:X321"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView showGridLines="0" zoomScale="183" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="3" width="12.85546875" customWidth="1"/>
-    <col min="5" max="6" width="14.7109375" customWidth="1"/>
-    <col min="7" max="8" width="10.7109375" customWidth="1"/>
+    <col min="2" max="3" width="12.83203125" customWidth="1"/>
+    <col min="5" max="6" width="14.6640625" customWidth="1"/>
+    <col min="7" max="8" width="10.6640625" customWidth="1"/>
     <col min="9" max="9" width="16" customWidth="1"/>
-    <col min="10" max="10" width="11.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.7109375" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="20" width="10.7109375" customWidth="1"/>
+    <col min="10" max="10" width="11.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.6640625" customWidth="1"/>
+    <col min="12" max="12" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="20" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B2" s="11" t="s">
+    <row r="2" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B2" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="H2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="K2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="O2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="11" t="s">
+      <c r="R2" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="R2" s="11" t="s">
+      <c r="V2" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="V2" s="11" t="s">
+    </row>
+    <row r="3" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B3" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B3" s="5" t="s">
-        <v>1</v>
+      <c r="H3" s="1" t="s">
+        <v>3</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>18</v>
+      <c r="I3" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="J3"/>
       <c r="K3" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
-      <c r="L3" s="8" t="s">
+      <c r="L3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="M3" s="1" t="s">
-        <v>5</v>
+      <c r="T3" s="1" t="s">
+        <v>4</v>
       </c>
-      <c r="O3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="P3" s="1" t="s">
+      <c r="V3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="R3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="V3" s="1" t="s">
+      <c r="W3" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="W3" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="X3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B4" s="5"/>
-      <c r="C4" s="4"/>
+    <row r="4" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B4" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="11">
+        <v>15106</v>
+      </c>
       <c r="E4" s="1"/>
-      <c r="F4" s="12"/>
+      <c r="F4" s="6"/>
       <c r="H4" s="1"/>
-      <c r="I4" s="8"/>
+      <c r="I4" s="6"/>
       <c r="J4"/>
       <c r="K4" s="1"/>
-      <c r="L4" s="8"/>
+      <c r="L4" s="6"/>
       <c r="M4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
@@ -6623,16 +6810,20 @@
       <c r="W4" s="1"/>
       <c r="X4" s="1"/>
     </row>
-    <row r="5" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B5" s="5"/>
-      <c r="C5" s="4"/>
+    <row r="5" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B5" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="11">
+        <v>10003</v>
+      </c>
       <c r="E5" s="1"/>
-      <c r="F5" s="8"/>
+      <c r="F5" s="6"/>
       <c r="H5" s="1"/>
-      <c r="I5" s="8"/>
+      <c r="I5" s="6"/>
       <c r="J5"/>
       <c r="K5" s="1"/>
-      <c r="L5" s="8"/>
+      <c r="L5" s="6"/>
       <c r="M5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
@@ -6643,14 +6834,14 @@
       <c r="W5" s="1"/>
       <c r="X5" s="1"/>
     </row>
-    <row r="6" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:24" x14ac:dyDescent="0.2">
       <c r="E6" s="1"/>
-      <c r="F6" s="8"/>
+      <c r="F6" s="6"/>
       <c r="H6" s="1"/>
-      <c r="I6" s="8"/>
+      <c r="I6" s="6"/>
       <c r="J6"/>
       <c r="K6" s="1"/>
-      <c r="L6" s="8"/>
+      <c r="L6" s="6"/>
       <c r="M6" s="1"/>
       <c r="R6" s="1"/>
       <c r="S6" s="2"/>
@@ -6659,14 +6850,14 @@
       <c r="W6" s="1"/>
       <c r="X6" s="1"/>
     </row>
-    <row r="7" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:24" x14ac:dyDescent="0.2">
       <c r="E7" s="1"/>
-      <c r="F7" s="8"/>
+      <c r="F7" s="6"/>
       <c r="H7" s="1"/>
-      <c r="I7" s="8"/>
+      <c r="I7" s="6"/>
       <c r="J7"/>
       <c r="K7" s="1"/>
-      <c r="L7" s="8"/>
+      <c r="L7" s="6"/>
       <c r="M7" s="1"/>
       <c r="R7" s="1"/>
       <c r="S7" s="2"/>
@@ -6675,14 +6866,14 @@
       <c r="W7" s="1"/>
       <c r="X7" s="1"/>
     </row>
-    <row r="8" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:24" x14ac:dyDescent="0.2">
       <c r="E8" s="1"/>
-      <c r="F8" s="8"/>
+      <c r="F8" s="6"/>
       <c r="H8" s="1"/>
-      <c r="I8" s="8"/>
+      <c r="I8" s="6"/>
       <c r="J8"/>
       <c r="K8" s="1"/>
-      <c r="L8" s="8"/>
+      <c r="L8" s="6"/>
       <c r="M8" s="1"/>
       <c r="R8" s="1"/>
       <c r="S8" s="2"/>
@@ -6691,9 +6882,9 @@
       <c r="W8" s="1"/>
       <c r="X8" s="1"/>
     </row>
-    <row r="9" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:24" x14ac:dyDescent="0.2">
       <c r="E9" s="1"/>
-      <c r="F9" s="8"/>
+      <c r="F9" s="6"/>
       <c r="J9"/>
       <c r="R9" s="1"/>
       <c r="S9" s="2"/>
@@ -6702,1585 +6893,1585 @@
       <c r="W9" s="1"/>
       <c r="X9" s="1"/>
     </row>
-    <row r="10" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:24" x14ac:dyDescent="0.2">
       <c r="E10" s="1"/>
-      <c r="F10" s="8"/>
+      <c r="F10" s="6"/>
       <c r="J10"/>
       <c r="V10" s="1"/>
       <c r="W10" s="1"/>
       <c r="X10" s="1"/>
     </row>
-    <row r="11" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:24" x14ac:dyDescent="0.2">
       <c r="E11" s="1"/>
-      <c r="F11" s="8"/>
+      <c r="F11" s="6"/>
       <c r="J11"/>
       <c r="V11" s="1"/>
       <c r="W11" s="1"/>
       <c r="X11" s="1"/>
     </row>
-    <row r="12" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:24" x14ac:dyDescent="0.2">
       <c r="V12" s="1"/>
       <c r="W12" s="1"/>
       <c r="X12" s="1"/>
     </row>
-    <row r="13" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:24" x14ac:dyDescent="0.2">
       <c r="V13" s="1"/>
       <c r="W13" s="1"/>
       <c r="X13" s="1"/>
     </row>
-    <row r="14" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:24" x14ac:dyDescent="0.2">
       <c r="V14" s="1"/>
       <c r="W14" s="1"/>
       <c r="X14" s="1"/>
     </row>
-    <row r="15" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:24" x14ac:dyDescent="0.2">
       <c r="V15" s="1"/>
       <c r="W15" s="1"/>
       <c r="X15" s="1"/>
     </row>
-    <row r="16" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:24" x14ac:dyDescent="0.2">
       <c r="V16" s="1"/>
       <c r="W16" s="1"/>
       <c r="X16" s="1"/>
     </row>
-    <row r="17" spans="4:24" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:24" x14ac:dyDescent="0.2">
       <c r="V17" s="1"/>
       <c r="W17" s="1"/>
       <c r="X17" s="1"/>
     </row>
-    <row r="18" spans="4:24" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:24" x14ac:dyDescent="0.2">
       <c r="V18" s="1"/>
       <c r="W18" s="1"/>
       <c r="X18" s="1"/>
     </row>
-    <row r="19" spans="4:24" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:24" x14ac:dyDescent="0.2">
       <c r="V19" s="1"/>
       <c r="W19" s="1"/>
       <c r="X19" s="1"/>
     </row>
-    <row r="20" spans="4:24" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:24" x14ac:dyDescent="0.2">
       <c r="V20" s="1"/>
       <c r="W20" s="1"/>
       <c r="X20" s="1"/>
     </row>
-    <row r="21" spans="4:24" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:24" x14ac:dyDescent="0.2">
       <c r="V21" s="1"/>
       <c r="W21" s="1"/>
       <c r="X21" s="1"/>
     </row>
-    <row r="22" spans="4:24" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:24" x14ac:dyDescent="0.2">
       <c r="V22" s="1"/>
       <c r="W22" s="1"/>
       <c r="X22" s="1"/>
     </row>
-    <row r="23" spans="4:24" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:24" x14ac:dyDescent="0.2">
       <c r="V23" s="1"/>
       <c r="W23" s="1"/>
       <c r="X23" s="1"/>
     </row>
-    <row r="24" spans="4:24" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:24" x14ac:dyDescent="0.2">
       <c r="V24" s="1"/>
       <c r="W24" s="1"/>
       <c r="X24" s="1"/>
     </row>
-    <row r="25" spans="4:24" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:24" x14ac:dyDescent="0.2">
       <c r="V25" s="1"/>
       <c r="W25" s="1"/>
       <c r="X25" s="1"/>
     </row>
-    <row r="26" spans="4:24" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:24" x14ac:dyDescent="0.2">
       <c r="V26" s="1"/>
       <c r="W26" s="1"/>
       <c r="X26" s="1"/>
     </row>
-    <row r="27" spans="4:24" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:24" x14ac:dyDescent="0.2">
       <c r="V27" s="1"/>
       <c r="W27" s="1"/>
       <c r="X27" s="1"/>
     </row>
-    <row r="28" spans="4:24" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:24" x14ac:dyDescent="0.2">
       <c r="D28" s="3"/>
       <c r="V28" s="1"/>
       <c r="W28" s="1"/>
       <c r="X28" s="1"/>
     </row>
-    <row r="29" spans="4:24" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:24" x14ac:dyDescent="0.2">
       <c r="D29" s="3"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="6"/>
-      <c r="J29" s="9"/>
-      <c r="K29" s="6"/>
-      <c r="L29" s="6"/>
-      <c r="M29" s="6"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="7"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="4"/>
+      <c r="M29" s="4"/>
       <c r="V29" s="1"/>
       <c r="W29" s="1"/>
       <c r="X29" s="1"/>
     </row>
-    <row r="30" spans="4:24" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:24" x14ac:dyDescent="0.2">
       <c r="D30" s="3"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="7"/>
-      <c r="I30" s="7"/>
-      <c r="J30" s="10"/>
-      <c r="K30" s="7"/>
-      <c r="L30" s="7"/>
-      <c r="M30" s="7"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="8"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="5"/>
+      <c r="M30" s="5"/>
       <c r="V30" s="1"/>
       <c r="W30" s="1"/>
       <c r="X30" s="1"/>
     </row>
-    <row r="31" spans="4:24" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:24" x14ac:dyDescent="0.2">
       <c r="V31" s="1"/>
       <c r="W31" s="1"/>
       <c r="X31" s="1"/>
     </row>
-    <row r="32" spans="4:24" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:24" x14ac:dyDescent="0.2">
       <c r="V32" s="1"/>
       <c r="W32" s="1"/>
       <c r="X32" s="1"/>
     </row>
-    <row r="33" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="33" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V33" s="1"/>
       <c r="W33" s="1"/>
       <c r="X33" s="1"/>
     </row>
-    <row r="34" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="34" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V34" s="1"/>
       <c r="W34" s="1"/>
       <c r="X34" s="1"/>
     </row>
-    <row r="35" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="35" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V35" s="1"/>
       <c r="W35" s="1"/>
       <c r="X35" s="1"/>
     </row>
-    <row r="36" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="36" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V36" s="1"/>
       <c r="W36" s="1"/>
       <c r="X36" s="1"/>
     </row>
-    <row r="37" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="37" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V37" s="1"/>
       <c r="W37" s="1"/>
       <c r="X37" s="1"/>
     </row>
-    <row r="38" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="38" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V38" s="1"/>
       <c r="W38" s="1"/>
       <c r="X38" s="1"/>
     </row>
-    <row r="39" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="39" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V39" s="1"/>
       <c r="W39" s="1"/>
       <c r="X39" s="1"/>
     </row>
-    <row r="40" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="40" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V40" s="1"/>
       <c r="W40" s="1"/>
       <c r="X40" s="1"/>
     </row>
-    <row r="41" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="41" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V41" s="1"/>
       <c r="W41" s="1"/>
       <c r="X41" s="1"/>
     </row>
-    <row r="42" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="42" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V42" s="1"/>
       <c r="W42" s="1"/>
       <c r="X42" s="1"/>
     </row>
-    <row r="43" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="43" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V43" s="1"/>
       <c r="W43" s="1"/>
       <c r="X43" s="1"/>
     </row>
-    <row r="44" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="44" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V44" s="1"/>
       <c r="W44" s="1"/>
       <c r="X44" s="1"/>
     </row>
-    <row r="45" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="45" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V45" s="1"/>
       <c r="W45" s="1"/>
       <c r="X45" s="1"/>
     </row>
-    <row r="46" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="46" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V46" s="1"/>
       <c r="W46" s="1"/>
       <c r="X46" s="1"/>
     </row>
-    <row r="47" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="47" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V47" s="1"/>
       <c r="W47" s="1"/>
       <c r="X47" s="1"/>
     </row>
-    <row r="48" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="48" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V48" s="1"/>
       <c r="W48" s="1"/>
       <c r="X48" s="1"/>
     </row>
-    <row r="49" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="49" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V49" s="1"/>
       <c r="W49" s="1"/>
       <c r="X49" s="1"/>
     </row>
-    <row r="50" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="50" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V50" s="1"/>
       <c r="W50" s="1"/>
       <c r="X50" s="1"/>
     </row>
-    <row r="51" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="51" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V51" s="1"/>
       <c r="W51" s="1"/>
       <c r="X51" s="1"/>
     </row>
-    <row r="52" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="52" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V52" s="1"/>
       <c r="W52" s="1"/>
       <c r="X52" s="1"/>
     </row>
-    <row r="53" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="53" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V53" s="1"/>
       <c r="W53" s="1"/>
       <c r="X53" s="1"/>
     </row>
-    <row r="54" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="54" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V54" s="1"/>
       <c r="W54" s="1"/>
       <c r="X54" s="1"/>
     </row>
-    <row r="55" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="55" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V55" s="1"/>
       <c r="W55" s="1"/>
       <c r="X55" s="1"/>
     </row>
-    <row r="56" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="56" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V56" s="1"/>
       <c r="W56" s="1"/>
       <c r="X56" s="1"/>
     </row>
-    <row r="57" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="57" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V57" s="1"/>
       <c r="W57" s="1"/>
       <c r="X57" s="1"/>
     </row>
-    <row r="58" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="58" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V58" s="1"/>
       <c r="W58" s="1"/>
       <c r="X58" s="1"/>
     </row>
-    <row r="59" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="59" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V59" s="1"/>
       <c r="W59" s="1"/>
       <c r="X59" s="1"/>
     </row>
-    <row r="60" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="60" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V60" s="1"/>
       <c r="W60" s="1"/>
       <c r="X60" s="1"/>
     </row>
-    <row r="61" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="61" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V61" s="1"/>
       <c r="W61" s="1"/>
       <c r="X61" s="1"/>
     </row>
-    <row r="62" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="62" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V62" s="1"/>
       <c r="W62" s="1"/>
       <c r="X62" s="1"/>
     </row>
-    <row r="63" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="63" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V63" s="1"/>
       <c r="W63" s="1"/>
       <c r="X63" s="1"/>
     </row>
-    <row r="64" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="64" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V64" s="1"/>
       <c r="W64" s="1"/>
       <c r="X64" s="1"/>
     </row>
-    <row r="65" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="65" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V65" s="1"/>
       <c r="W65" s="1"/>
       <c r="X65" s="1"/>
     </row>
-    <row r="66" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="66" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V66" s="1"/>
       <c r="W66" s="1"/>
       <c r="X66" s="1"/>
     </row>
-    <row r="67" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="67" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V67" s="1"/>
       <c r="W67" s="1"/>
       <c r="X67" s="1"/>
     </row>
-    <row r="68" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="68" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V68" s="1"/>
       <c r="W68" s="1"/>
       <c r="X68" s="1"/>
     </row>
-    <row r="69" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="69" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V69" s="1"/>
       <c r="W69" s="1"/>
       <c r="X69" s="1"/>
     </row>
-    <row r="70" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="70" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V70" s="1"/>
       <c r="W70" s="1"/>
       <c r="X70" s="1"/>
     </row>
-    <row r="71" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="71" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V71" s="1"/>
       <c r="W71" s="1"/>
       <c r="X71" s="1"/>
     </row>
-    <row r="72" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="72" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V72" s="1"/>
       <c r="W72" s="1"/>
       <c r="X72" s="1"/>
     </row>
-    <row r="73" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="73" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V73" s="1"/>
       <c r="W73" s="1"/>
       <c r="X73" s="1"/>
     </row>
-    <row r="74" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="74" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V74" s="1"/>
       <c r="W74" s="1"/>
       <c r="X74" s="1"/>
     </row>
-    <row r="75" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="75" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V75" s="1"/>
       <c r="W75" s="1"/>
       <c r="X75" s="1"/>
     </row>
-    <row r="76" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="76" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V76" s="1"/>
       <c r="W76" s="1"/>
       <c r="X76" s="1"/>
     </row>
-    <row r="77" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="77" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V77" s="1"/>
       <c r="W77" s="1"/>
       <c r="X77" s="1"/>
     </row>
-    <row r="78" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="78" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V78" s="1"/>
       <c r="W78" s="1"/>
       <c r="X78" s="1"/>
     </row>
-    <row r="79" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="79" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V79" s="1"/>
       <c r="W79" s="1"/>
       <c r="X79" s="1"/>
     </row>
-    <row r="80" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="80" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V80" s="1"/>
       <c r="W80" s="1"/>
       <c r="X80" s="1"/>
     </row>
-    <row r="81" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="81" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V81" s="1"/>
       <c r="W81" s="1"/>
       <c r="X81" s="1"/>
     </row>
-    <row r="82" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="82" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V82" s="1"/>
       <c r="W82" s="1"/>
       <c r="X82" s="1"/>
     </row>
-    <row r="83" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="83" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V83" s="1"/>
       <c r="W83" s="1"/>
       <c r="X83" s="1"/>
     </row>
-    <row r="84" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="84" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V84" s="1"/>
       <c r="W84" s="1"/>
       <c r="X84" s="1"/>
     </row>
-    <row r="85" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="85" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V85" s="1"/>
       <c r="W85" s="1"/>
       <c r="X85" s="1"/>
     </row>
-    <row r="86" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="86" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V86" s="1"/>
       <c r="W86" s="1"/>
       <c r="X86" s="1"/>
     </row>
-    <row r="87" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="87" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V87" s="1"/>
       <c r="W87" s="1"/>
       <c r="X87" s="1"/>
     </row>
-    <row r="88" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="88" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V88" s="1"/>
       <c r="W88" s="1"/>
       <c r="X88" s="1"/>
     </row>
-    <row r="89" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="89" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V89" s="1"/>
       <c r="W89" s="1"/>
       <c r="X89" s="1"/>
     </row>
-    <row r="90" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="90" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V90" s="1"/>
       <c r="W90" s="1"/>
       <c r="X90" s="1"/>
     </row>
-    <row r="91" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="91" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V91" s="1"/>
       <c r="W91" s="1"/>
       <c r="X91" s="1"/>
     </row>
-    <row r="92" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="92" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V92" s="1"/>
       <c r="W92" s="1"/>
       <c r="X92" s="1"/>
     </row>
-    <row r="93" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="93" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V93" s="1"/>
       <c r="W93" s="1"/>
       <c r="X93" s="1"/>
     </row>
-    <row r="94" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="94" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V94" s="1"/>
       <c r="W94" s="1"/>
       <c r="X94" s="1"/>
     </row>
-    <row r="95" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="95" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V95" s="1"/>
       <c r="W95" s="1"/>
       <c r="X95" s="1"/>
     </row>
-    <row r="96" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="96" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V96" s="1"/>
       <c r="W96" s="1"/>
       <c r="X96" s="1"/>
     </row>
-    <row r="97" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="97" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V97" s="1"/>
       <c r="W97" s="1"/>
       <c r="X97" s="1"/>
     </row>
-    <row r="98" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="98" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V98" s="1"/>
       <c r="W98" s="1"/>
       <c r="X98" s="1"/>
     </row>
-    <row r="99" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="99" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V99" s="1"/>
       <c r="W99" s="1"/>
       <c r="X99" s="1"/>
     </row>
-    <row r="100" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="100" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V100" s="1"/>
       <c r="W100" s="1"/>
       <c r="X100" s="1"/>
     </row>
-    <row r="101" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="101" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V101" s="1"/>
       <c r="W101" s="1"/>
       <c r="X101" s="1"/>
     </row>
-    <row r="102" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="102" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V102" s="1"/>
       <c r="W102" s="1"/>
       <c r="X102" s="1"/>
     </row>
-    <row r="103" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="103" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V103" s="1"/>
       <c r="W103" s="1"/>
       <c r="X103" s="1"/>
     </row>
-    <row r="104" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="104" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V104" s="1"/>
       <c r="W104" s="1"/>
       <c r="X104" s="1"/>
     </row>
-    <row r="105" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="105" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V105" s="1"/>
       <c r="W105" s="1"/>
       <c r="X105" s="1"/>
     </row>
-    <row r="106" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="106" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V106" s="1"/>
       <c r="W106" s="1"/>
       <c r="X106" s="1"/>
     </row>
-    <row r="107" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="107" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V107" s="1"/>
       <c r="W107" s="1"/>
       <c r="X107" s="1"/>
     </row>
-    <row r="108" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="108" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V108" s="1"/>
       <c r="W108" s="1"/>
       <c r="X108" s="1"/>
     </row>
-    <row r="109" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="109" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V109" s="1"/>
       <c r="W109" s="1"/>
       <c r="X109" s="1"/>
     </row>
-    <row r="110" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="110" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V110" s="1"/>
       <c r="W110" s="1"/>
       <c r="X110" s="1"/>
     </row>
-    <row r="111" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="111" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V111" s="1"/>
       <c r="W111" s="1"/>
       <c r="X111" s="1"/>
     </row>
-    <row r="112" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="112" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V112" s="1"/>
       <c r="W112" s="1"/>
       <c r="X112" s="1"/>
     </row>
-    <row r="113" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="113" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V113" s="1"/>
       <c r="W113" s="1"/>
       <c r="X113" s="1"/>
     </row>
-    <row r="114" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="114" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V114" s="1"/>
       <c r="W114" s="1"/>
       <c r="X114" s="1"/>
     </row>
-    <row r="115" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="115" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V115" s="1"/>
       <c r="W115" s="1"/>
       <c r="X115" s="1"/>
     </row>
-    <row r="116" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="116" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V116" s="1"/>
       <c r="W116" s="1"/>
       <c r="X116" s="1"/>
     </row>
-    <row r="117" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="117" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V117" s="1"/>
       <c r="W117" s="1"/>
       <c r="X117" s="1"/>
     </row>
-    <row r="118" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="118" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V118" s="1"/>
       <c r="W118" s="1"/>
       <c r="X118" s="1"/>
     </row>
-    <row r="119" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="119" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V119" s="1"/>
       <c r="W119" s="1"/>
       <c r="X119" s="1"/>
     </row>
-    <row r="120" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="120" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V120" s="1"/>
       <c r="W120" s="1"/>
       <c r="X120" s="1"/>
     </row>
-    <row r="121" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="121" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V121" s="1"/>
       <c r="W121" s="1"/>
       <c r="X121" s="1"/>
     </row>
-    <row r="122" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="122" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V122" s="1"/>
       <c r="W122" s="1"/>
       <c r="X122" s="1"/>
     </row>
-    <row r="123" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="123" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V123" s="1"/>
       <c r="W123" s="1"/>
       <c r="X123" s="1"/>
     </row>
-    <row r="124" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="124" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V124" s="1"/>
       <c r="W124" s="1"/>
       <c r="X124" s="1"/>
     </row>
-    <row r="125" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="125" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V125" s="1"/>
       <c r="W125" s="1"/>
       <c r="X125" s="1"/>
     </row>
-    <row r="126" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="126" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V126" s="1"/>
       <c r="W126" s="1"/>
       <c r="X126" s="1"/>
     </row>
-    <row r="127" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="127" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V127" s="1"/>
       <c r="W127" s="1"/>
       <c r="X127" s="1"/>
     </row>
-    <row r="128" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="128" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V128" s="1"/>
       <c r="W128" s="1"/>
       <c r="X128" s="1"/>
     </row>
-    <row r="129" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="129" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V129" s="1"/>
       <c r="W129" s="1"/>
       <c r="X129" s="1"/>
     </row>
-    <row r="130" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="130" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V130" s="1"/>
       <c r="W130" s="1"/>
       <c r="X130" s="1"/>
     </row>
-    <row r="131" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="131" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V131" s="1"/>
       <c r="W131" s="1"/>
       <c r="X131" s="1"/>
     </row>
-    <row r="132" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="132" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V132" s="1"/>
       <c r="W132" s="1"/>
       <c r="X132" s="1"/>
     </row>
-    <row r="133" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="133" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V133" s="1"/>
       <c r="W133" s="1"/>
       <c r="X133" s="1"/>
     </row>
-    <row r="134" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="134" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V134" s="1"/>
       <c r="W134" s="1"/>
       <c r="X134" s="1"/>
     </row>
-    <row r="135" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="135" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V135" s="1"/>
       <c r="W135" s="1"/>
       <c r="X135" s="1"/>
     </row>
-    <row r="136" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="136" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V136" s="1"/>
       <c r="W136" s="1"/>
       <c r="X136" s="1"/>
     </row>
-    <row r="137" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="137" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V137" s="1"/>
       <c r="W137" s="1"/>
       <c r="X137" s="1"/>
     </row>
-    <row r="138" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="138" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V138" s="1"/>
       <c r="W138" s="1"/>
       <c r="X138" s="1"/>
     </row>
-    <row r="139" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="139" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V139" s="1"/>
       <c r="W139" s="1"/>
       <c r="X139" s="1"/>
     </row>
-    <row r="140" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="140" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V140" s="1"/>
       <c r="W140" s="1"/>
       <c r="X140" s="1"/>
     </row>
-    <row r="141" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="141" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V141" s="1"/>
       <c r="W141" s="1"/>
       <c r="X141" s="1"/>
     </row>
-    <row r="142" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="142" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V142" s="1"/>
       <c r="W142" s="1"/>
       <c r="X142" s="1"/>
     </row>
-    <row r="143" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="143" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V143" s="1"/>
       <c r="W143" s="1"/>
       <c r="X143" s="1"/>
     </row>
-    <row r="144" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="144" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V144" s="1"/>
       <c r="W144" s="1"/>
       <c r="X144" s="1"/>
     </row>
-    <row r="145" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="145" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V145" s="1"/>
       <c r="W145" s="1"/>
       <c r="X145" s="1"/>
     </row>
-    <row r="146" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="146" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V146" s="1"/>
       <c r="W146" s="1"/>
       <c r="X146" s="1"/>
     </row>
-    <row r="147" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="147" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V147" s="1"/>
       <c r="W147" s="1"/>
       <c r="X147" s="1"/>
     </row>
-    <row r="148" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="148" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V148" s="1"/>
       <c r="W148" s="1"/>
       <c r="X148" s="1"/>
     </row>
-    <row r="149" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="149" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V149" s="1"/>
       <c r="W149" s="1"/>
       <c r="X149" s="1"/>
     </row>
-    <row r="150" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="150" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V150" s="1"/>
       <c r="W150" s="1"/>
       <c r="X150" s="1"/>
     </row>
-    <row r="151" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="151" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V151" s="1"/>
       <c r="W151" s="1"/>
       <c r="X151" s="1"/>
     </row>
-    <row r="152" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="152" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V152" s="1"/>
       <c r="W152" s="1"/>
       <c r="X152" s="1"/>
     </row>
-    <row r="153" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="153" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V153" s="1"/>
       <c r="W153" s="1"/>
       <c r="X153" s="1"/>
     </row>
-    <row r="154" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="154" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V154" s="1"/>
       <c r="W154" s="1"/>
       <c r="X154" s="1"/>
     </row>
-    <row r="155" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="155" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V155" s="1"/>
       <c r="W155" s="1"/>
       <c r="X155" s="1"/>
     </row>
-    <row r="156" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="156" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V156" s="1"/>
       <c r="W156" s="1"/>
       <c r="X156" s="1"/>
     </row>
-    <row r="157" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="157" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V157" s="1"/>
       <c r="W157" s="1"/>
       <c r="X157" s="1"/>
     </row>
-    <row r="158" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="158" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V158" s="1"/>
       <c r="W158" s="1"/>
       <c r="X158" s="1"/>
     </row>
-    <row r="159" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="159" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V159" s="1"/>
       <c r="W159" s="1"/>
       <c r="X159" s="1"/>
     </row>
-    <row r="160" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="160" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V160" s="1"/>
       <c r="W160" s="1"/>
       <c r="X160" s="1"/>
     </row>
-    <row r="161" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="161" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V161" s="1"/>
       <c r="W161" s="1"/>
       <c r="X161" s="1"/>
     </row>
-    <row r="162" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="162" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V162" s="1"/>
       <c r="W162" s="1"/>
       <c r="X162" s="1"/>
     </row>
-    <row r="163" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="163" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V163" s="1"/>
       <c r="W163" s="1"/>
       <c r="X163" s="1"/>
     </row>
-    <row r="164" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="164" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V164" s="1"/>
       <c r="W164" s="1"/>
       <c r="X164" s="1"/>
     </row>
-    <row r="165" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="165" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V165" s="1"/>
       <c r="W165" s="1"/>
       <c r="X165" s="1"/>
     </row>
-    <row r="166" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="166" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V166" s="1"/>
       <c r="W166" s="1"/>
       <c r="X166" s="1"/>
     </row>
-    <row r="167" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="167" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V167" s="1"/>
       <c r="W167" s="1"/>
       <c r="X167" s="1"/>
     </row>
-    <row r="168" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="168" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V168" s="1"/>
       <c r="W168" s="1"/>
       <c r="X168" s="1"/>
     </row>
-    <row r="169" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="169" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V169" s="1"/>
       <c r="W169" s="1"/>
       <c r="X169" s="1"/>
     </row>
-    <row r="170" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="170" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V170" s="1"/>
       <c r="W170" s="1"/>
       <c r="X170" s="1"/>
     </row>
-    <row r="171" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="171" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V171" s="1"/>
       <c r="W171" s="1"/>
       <c r="X171" s="1"/>
     </row>
-    <row r="172" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="172" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V172" s="1"/>
       <c r="W172" s="1"/>
       <c r="X172" s="1"/>
     </row>
-    <row r="173" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="173" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V173" s="1"/>
       <c r="W173" s="1"/>
       <c r="X173" s="1"/>
     </row>
-    <row r="174" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="174" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V174" s="1"/>
       <c r="W174" s="1"/>
       <c r="X174" s="1"/>
     </row>
-    <row r="175" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="175" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V175" s="1"/>
       <c r="W175" s="1"/>
       <c r="X175" s="1"/>
     </row>
-    <row r="176" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="176" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V176" s="1"/>
       <c r="W176" s="1"/>
       <c r="X176" s="1"/>
     </row>
-    <row r="177" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="177" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V177" s="1"/>
       <c r="W177" s="1"/>
       <c r="X177" s="1"/>
     </row>
-    <row r="178" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="178" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V178" s="1"/>
       <c r="W178" s="1"/>
       <c r="X178" s="1"/>
     </row>
-    <row r="179" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="179" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V179" s="1"/>
       <c r="W179" s="1"/>
       <c r="X179" s="1"/>
     </row>
-    <row r="180" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="180" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V180" s="1"/>
       <c r="W180" s="1"/>
       <c r="X180" s="1"/>
     </row>
-    <row r="181" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="181" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V181" s="1"/>
       <c r="W181" s="1"/>
       <c r="X181" s="1"/>
     </row>
-    <row r="182" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="182" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V182" s="1"/>
       <c r="W182" s="1"/>
       <c r="X182" s="1"/>
     </row>
-    <row r="183" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="183" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V183" s="1"/>
       <c r="W183" s="1"/>
       <c r="X183" s="1"/>
     </row>
-    <row r="184" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="184" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V184" s="1"/>
       <c r="W184" s="1"/>
       <c r="X184" s="1"/>
     </row>
-    <row r="185" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="185" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V185" s="1"/>
       <c r="W185" s="1"/>
       <c r="X185" s="1"/>
     </row>
-    <row r="186" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="186" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V186" s="1"/>
       <c r="W186" s="1"/>
       <c r="X186" s="1"/>
     </row>
-    <row r="187" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="187" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V187" s="1"/>
       <c r="W187" s="1"/>
       <c r="X187" s="1"/>
     </row>
-    <row r="188" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="188" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V188" s="1"/>
       <c r="W188" s="1"/>
       <c r="X188" s="1"/>
     </row>
-    <row r="189" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="189" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V189" s="1"/>
       <c r="W189" s="1"/>
       <c r="X189" s="1"/>
     </row>
-    <row r="190" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="190" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V190" s="1"/>
       <c r="W190" s="1"/>
       <c r="X190" s="1"/>
     </row>
-    <row r="191" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="191" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V191" s="1"/>
       <c r="W191" s="1"/>
       <c r="X191" s="1"/>
     </row>
-    <row r="192" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="192" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V192" s="1"/>
       <c r="W192" s="1"/>
       <c r="X192" s="1"/>
     </row>
-    <row r="193" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="193" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V193" s="1"/>
       <c r="W193" s="1"/>
       <c r="X193" s="1"/>
     </row>
-    <row r="194" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="194" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V194" s="1"/>
       <c r="W194" s="1"/>
       <c r="X194" s="1"/>
     </row>
-    <row r="195" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="195" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V195" s="1"/>
       <c r="W195" s="1"/>
       <c r="X195" s="1"/>
     </row>
-    <row r="196" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="196" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V196" s="1"/>
       <c r="W196" s="1"/>
       <c r="X196" s="1"/>
     </row>
-    <row r="197" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="197" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V197" s="1"/>
       <c r="W197" s="1"/>
       <c r="X197" s="1"/>
     </row>
-    <row r="198" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="198" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V198" s="1"/>
       <c r="W198" s="1"/>
       <c r="X198" s="1"/>
     </row>
-    <row r="199" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="199" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V199" s="1"/>
       <c r="W199" s="1"/>
       <c r="X199" s="1"/>
     </row>
-    <row r="200" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="200" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V200" s="1"/>
       <c r="W200" s="1"/>
       <c r="X200" s="1"/>
     </row>
-    <row r="201" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="201" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V201" s="1"/>
       <c r="W201" s="1"/>
       <c r="X201" s="1"/>
     </row>
-    <row r="202" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="202" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V202" s="1"/>
       <c r="W202" s="1"/>
       <c r="X202" s="1"/>
     </row>
-    <row r="203" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="203" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V203" s="1"/>
       <c r="W203" s="1"/>
       <c r="X203" s="1"/>
     </row>
-    <row r="204" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="204" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V204" s="1"/>
       <c r="W204" s="1"/>
       <c r="X204" s="1"/>
     </row>
-    <row r="205" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="205" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V205" s="1"/>
       <c r="W205" s="1"/>
       <c r="X205" s="1"/>
     </row>
-    <row r="206" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="206" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V206" s="1"/>
       <c r="W206" s="1"/>
       <c r="X206" s="1"/>
     </row>
-    <row r="207" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="207" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V207" s="1"/>
       <c r="W207" s="1"/>
       <c r="X207" s="1"/>
     </row>
-    <row r="208" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="208" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V208" s="1"/>
       <c r="W208" s="1"/>
       <c r="X208" s="1"/>
     </row>
-    <row r="209" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="209" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V209" s="1"/>
       <c r="W209" s="1"/>
       <c r="X209" s="1"/>
     </row>
-    <row r="210" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="210" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V210" s="1"/>
       <c r="W210" s="1"/>
       <c r="X210" s="1"/>
     </row>
-    <row r="211" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="211" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V211" s="1"/>
       <c r="W211" s="1"/>
       <c r="X211" s="1"/>
     </row>
-    <row r="212" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="212" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V212" s="1"/>
       <c r="W212" s="1"/>
       <c r="X212" s="1"/>
     </row>
-    <row r="213" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="213" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V213" s="1"/>
       <c r="W213" s="1"/>
       <c r="X213" s="1"/>
     </row>
-    <row r="214" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="214" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V214" s="1"/>
       <c r="W214" s="1"/>
       <c r="X214" s="1"/>
     </row>
-    <row r="215" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="215" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V215" s="1"/>
       <c r="W215" s="1"/>
       <c r="X215" s="1"/>
     </row>
-    <row r="216" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="216" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V216" s="1"/>
       <c r="W216" s="1"/>
       <c r="X216" s="1"/>
     </row>
-    <row r="217" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="217" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V217" s="1"/>
       <c r="W217" s="1"/>
       <c r="X217" s="1"/>
     </row>
-    <row r="218" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="218" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V218" s="1"/>
       <c r="W218" s="1"/>
       <c r="X218" s="1"/>
     </row>
-    <row r="219" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="219" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V219" s="1"/>
       <c r="W219" s="1"/>
       <c r="X219" s="1"/>
     </row>
-    <row r="220" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="220" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V220" s="1"/>
       <c r="W220" s="1"/>
       <c r="X220" s="1"/>
     </row>
-    <row r="221" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="221" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V221" s="1"/>
       <c r="W221" s="1"/>
       <c r="X221" s="1"/>
     </row>
-    <row r="222" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="222" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V222" s="1"/>
       <c r="W222" s="1"/>
       <c r="X222" s="1"/>
     </row>
-    <row r="223" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="223" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V223" s="1"/>
       <c r="W223" s="1"/>
       <c r="X223" s="1"/>
     </row>
-    <row r="224" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="224" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V224" s="1"/>
       <c r="W224" s="1"/>
       <c r="X224" s="1"/>
     </row>
-    <row r="225" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="225" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V225" s="1"/>
       <c r="W225" s="1"/>
       <c r="X225" s="1"/>
     </row>
-    <row r="226" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="226" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V226" s="1"/>
       <c r="W226" s="1"/>
       <c r="X226" s="1"/>
     </row>
-    <row r="227" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="227" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V227" s="1"/>
       <c r="W227" s="1"/>
       <c r="X227" s="1"/>
     </row>
-    <row r="228" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="228" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V228" s="1"/>
       <c r="W228" s="1"/>
       <c r="X228" s="1"/>
     </row>
-    <row r="229" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="229" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V229" s="1"/>
       <c r="W229" s="1"/>
       <c r="X229" s="1"/>
     </row>
-    <row r="230" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="230" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V230" s="1"/>
       <c r="W230" s="1"/>
       <c r="X230" s="1"/>
     </row>
-    <row r="231" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="231" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V231" s="1"/>
       <c r="W231" s="1"/>
       <c r="X231" s="1"/>
     </row>
-    <row r="232" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="232" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V232" s="1"/>
       <c r="W232" s="1"/>
       <c r="X232" s="1"/>
     </row>
-    <row r="233" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="233" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V233" s="1"/>
       <c r="W233" s="1"/>
       <c r="X233" s="1"/>
     </row>
-    <row r="234" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="234" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V234" s="1"/>
       <c r="W234" s="1"/>
       <c r="X234" s="1"/>
     </row>
-    <row r="235" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="235" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V235" s="1"/>
       <c r="W235" s="1"/>
       <c r="X235" s="1"/>
     </row>
-    <row r="236" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="236" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V236" s="1"/>
       <c r="W236" s="1"/>
       <c r="X236" s="1"/>
     </row>
-    <row r="237" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="237" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V237" s="1"/>
       <c r="W237" s="1"/>
       <c r="X237" s="1"/>
     </row>
-    <row r="238" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="238" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V238" s="1"/>
       <c r="W238" s="1"/>
       <c r="X238" s="1"/>
     </row>
-    <row r="239" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="239" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V239" s="1"/>
       <c r="W239" s="1"/>
       <c r="X239" s="1"/>
     </row>
-    <row r="240" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="240" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V240" s="1"/>
       <c r="W240" s="1"/>
       <c r="X240" s="1"/>
     </row>
-    <row r="241" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="241" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V241" s="1"/>
       <c r="W241" s="1"/>
       <c r="X241" s="1"/>
     </row>
-    <row r="242" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="242" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V242" s="1"/>
       <c r="W242" s="1"/>
       <c r="X242" s="1"/>
     </row>
-    <row r="243" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="243" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V243" s="1"/>
       <c r="W243" s="1"/>
       <c r="X243" s="1"/>
     </row>
-    <row r="244" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="244" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V244" s="1"/>
       <c r="W244" s="1"/>
       <c r="X244" s="1"/>
     </row>
-    <row r="245" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="245" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V245" s="1"/>
       <c r="W245" s="1"/>
       <c r="X245" s="1"/>
     </row>
-    <row r="246" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="246" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V246" s="1"/>
       <c r="W246" s="1"/>
       <c r="X246" s="1"/>
     </row>
-    <row r="247" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="247" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V247" s="1"/>
       <c r="W247" s="1"/>
       <c r="X247" s="1"/>
     </row>
-    <row r="248" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="248" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V248" s="1"/>
       <c r="W248" s="1"/>
       <c r="X248" s="1"/>
     </row>
-    <row r="249" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="249" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V249" s="1"/>
       <c r="W249" s="1"/>
       <c r="X249" s="1"/>
     </row>
-    <row r="250" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="250" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V250" s="1"/>
       <c r="W250" s="1"/>
       <c r="X250" s="1"/>
     </row>
-    <row r="251" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="251" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V251" s="1"/>
       <c r="W251" s="1"/>
       <c r="X251" s="1"/>
     </row>
-    <row r="252" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="252" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V252" s="1"/>
       <c r="W252" s="1"/>
       <c r="X252" s="1"/>
     </row>
-    <row r="253" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="253" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V253" s="1"/>
       <c r="W253" s="1"/>
       <c r="X253" s="1"/>
     </row>
-    <row r="254" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="254" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V254" s="1"/>
       <c r="W254" s="1"/>
       <c r="X254" s="1"/>
     </row>
-    <row r="255" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="255" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V255" s="1"/>
       <c r="W255" s="1"/>
       <c r="X255" s="1"/>
     </row>
-    <row r="256" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="256" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V256" s="1"/>
       <c r="W256" s="1"/>
       <c r="X256" s="1"/>
     </row>
-    <row r="257" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="257" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V257" s="1"/>
       <c r="W257" s="1"/>
       <c r="X257" s="1"/>
     </row>
-    <row r="258" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="258" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V258" s="1"/>
       <c r="W258" s="1"/>
       <c r="X258" s="1"/>
     </row>
-    <row r="259" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="259" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V259" s="1"/>
       <c r="W259" s="1"/>
       <c r="X259" s="1"/>
     </row>
-    <row r="260" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="260" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V260" s="1"/>
       <c r="W260" s="1"/>
       <c r="X260" s="1"/>
     </row>
-    <row r="261" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="261" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V261" s="1"/>
       <c r="W261" s="1"/>
       <c r="X261" s="1"/>
     </row>
-    <row r="262" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="262" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V262" s="1"/>
       <c r="W262" s="1"/>
       <c r="X262" s="1"/>
     </row>
-    <row r="263" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="263" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V263" s="1"/>
       <c r="W263" s="1"/>
       <c r="X263" s="1"/>
     </row>
-    <row r="264" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="264" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V264" s="1"/>
       <c r="W264" s="1"/>
       <c r="X264" s="1"/>
     </row>
-    <row r="265" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="265" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V265" s="1"/>
       <c r="W265" s="1"/>
       <c r="X265" s="1"/>
     </row>
-    <row r="266" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="266" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V266" s="1"/>
       <c r="W266" s="1"/>
       <c r="X266" s="1"/>
     </row>
-    <row r="267" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="267" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V267" s="1"/>
       <c r="W267" s="1"/>
       <c r="X267" s="1"/>
     </row>
-    <row r="268" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="268" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V268" s="1"/>
       <c r="W268" s="1"/>
       <c r="X268" s="1"/>
     </row>
-    <row r="269" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="269" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V269" s="1"/>
       <c r="W269" s="1"/>
       <c r="X269" s="1"/>
     </row>
-    <row r="270" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="270" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V270" s="1"/>
       <c r="W270" s="1"/>
       <c r="X270" s="1"/>
     </row>
-    <row r="271" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="271" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V271" s="1"/>
       <c r="W271" s="1"/>
       <c r="X271" s="1"/>
     </row>
-    <row r="272" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="272" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V272" s="1"/>
       <c r="W272" s="1"/>
       <c r="X272" s="1"/>
     </row>
-    <row r="273" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="273" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V273" s="1"/>
       <c r="W273" s="1"/>
       <c r="X273" s="1"/>
     </row>
-    <row r="274" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="274" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V274" s="1"/>
       <c r="W274" s="1"/>
       <c r="X274" s="1"/>
     </row>
-    <row r="275" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="275" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V275" s="1"/>
       <c r="W275" s="1"/>
       <c r="X275" s="1"/>
     </row>
-    <row r="276" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="276" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V276" s="1"/>
       <c r="W276" s="1"/>
       <c r="X276" s="1"/>
     </row>
-    <row r="277" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="277" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V277" s="1"/>
       <c r="W277" s="1"/>
       <c r="X277" s="1"/>
     </row>
-    <row r="278" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="278" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V278" s="1"/>
       <c r="W278" s="1"/>
       <c r="X278" s="1"/>
     </row>
-    <row r="279" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="279" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V279" s="1"/>
       <c r="W279" s="1"/>
       <c r="X279" s="1"/>
     </row>
-    <row r="280" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="280" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V280" s="1"/>
       <c r="W280" s="1"/>
       <c r="X280" s="1"/>
     </row>
-    <row r="281" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="281" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V281" s="1"/>
       <c r="W281" s="1"/>
       <c r="X281" s="1"/>
     </row>
-    <row r="282" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="282" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V282" s="1"/>
       <c r="W282" s="1"/>
       <c r="X282" s="1"/>
     </row>
-    <row r="283" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="283" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V283" s="1"/>
       <c r="W283" s="1"/>
       <c r="X283" s="1"/>
     </row>
-    <row r="284" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="284" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V284" s="1"/>
       <c r="W284" s="1"/>
       <c r="X284" s="1"/>
     </row>
-    <row r="285" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="285" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V285" s="1"/>
       <c r="W285" s="1"/>
       <c r="X285" s="1"/>
     </row>
-    <row r="286" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="286" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V286" s="1"/>
       <c r="W286" s="1"/>
       <c r="X286" s="1"/>
     </row>
-    <row r="287" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="287" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V287" s="1"/>
       <c r="W287" s="1"/>
       <c r="X287" s="1"/>
     </row>
-    <row r="288" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="288" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V288" s="1"/>
       <c r="W288" s="1"/>
       <c r="X288" s="1"/>
     </row>
-    <row r="289" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="289" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V289" s="1"/>
       <c r="W289" s="1"/>
       <c r="X289" s="1"/>
     </row>
-    <row r="290" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="290" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V290" s="1"/>
       <c r="W290" s="1"/>
       <c r="X290" s="1"/>
     </row>
-    <row r="291" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="291" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V291" s="1"/>
       <c r="W291" s="1"/>
       <c r="X291" s="1"/>
     </row>
-    <row r="292" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="292" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V292" s="1"/>
       <c r="W292" s="1"/>
       <c r="X292" s="1"/>
     </row>
-    <row r="293" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="293" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V293" s="1"/>
       <c r="W293" s="1"/>
       <c r="X293" s="1"/>
     </row>
-    <row r="294" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="294" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V294" s="1"/>
       <c r="W294" s="1"/>
       <c r="X294" s="1"/>
     </row>
-    <row r="295" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="295" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V295" s="1"/>
       <c r="W295" s="1"/>
       <c r="X295" s="1"/>
     </row>
-    <row r="296" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="296" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V296" s="1"/>
       <c r="W296" s="1"/>
       <c r="X296" s="1"/>
     </row>
-    <row r="297" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="297" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V297" s="1"/>
       <c r="W297" s="1"/>
       <c r="X297" s="1"/>
     </row>
-    <row r="298" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="298" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V298" s="1"/>
       <c r="W298" s="1"/>
       <c r="X298" s="1"/>
     </row>
-    <row r="299" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="299" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V299" s="1"/>
       <c r="W299" s="1"/>
       <c r="X299" s="1"/>
     </row>
-    <row r="300" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="300" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V300" s="1"/>
       <c r="W300" s="1"/>
       <c r="X300" s="1"/>
     </row>
-    <row r="301" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="301" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V301" s="1"/>
       <c r="W301" s="1"/>
       <c r="X301" s="1"/>
     </row>
-    <row r="302" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="302" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V302" s="1"/>
       <c r="W302" s="1"/>
       <c r="X302" s="1"/>
     </row>
-    <row r="303" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="303" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V303" s="1"/>
       <c r="W303" s="1"/>
       <c r="X303" s="1"/>
     </row>
-    <row r="304" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="304" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V304" s="1"/>
       <c r="W304" s="1"/>
       <c r="X304" s="1"/>
     </row>
-    <row r="305" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="305" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V305" s="1"/>
       <c r="W305" s="1"/>
       <c r="X305" s="1"/>
     </row>
-    <row r="306" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="306" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V306" s="1"/>
       <c r="W306" s="1"/>
       <c r="X306" s="1"/>
     </row>
-    <row r="307" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="307" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V307" s="1"/>
       <c r="W307" s="1"/>
       <c r="X307" s="1"/>
     </row>
-    <row r="308" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="308" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V308" s="1"/>
       <c r="W308" s="1"/>
       <c r="X308" s="1"/>
     </row>
-    <row r="309" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="309" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V309" s="1"/>
       <c r="W309" s="1"/>
       <c r="X309" s="1"/>
     </row>
-    <row r="310" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="310" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V310" s="1"/>
       <c r="W310" s="1"/>
       <c r="X310" s="1"/>
     </row>
-    <row r="311" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="311" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V311" s="1"/>
       <c r="W311" s="1"/>
       <c r="X311" s="1"/>
     </row>
-    <row r="312" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="312" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V312" s="1"/>
       <c r="W312" s="1"/>
       <c r="X312" s="1"/>
     </row>
-    <row r="313" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="313" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V313" s="1"/>
       <c r="W313" s="1"/>
       <c r="X313" s="1"/>
     </row>
-    <row r="314" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="314" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V314" s="1"/>
       <c r="W314" s="1"/>
       <c r="X314" s="1"/>
     </row>
-    <row r="315" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="315" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V315" s="1"/>
       <c r="W315" s="1"/>
       <c r="X315" s="1"/>
     </row>
-    <row r="316" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="316" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V316" s="1"/>
       <c r="W316" s="1"/>
       <c r="X316" s="1"/>
     </row>
-    <row r="317" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="317" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V317" s="1"/>
       <c r="W317" s="1"/>
       <c r="X317" s="1"/>
     </row>
-    <row r="318" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="318" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V318" s="1"/>
       <c r="W318" s="1"/>
       <c r="X318" s="1"/>
     </row>
-    <row r="319" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="319" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V319" s="1"/>
       <c r="W319" s="1"/>
       <c r="X319" s="1"/>
     </row>
-    <row r="320" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="320" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V320" s="1"/>
       <c r="W320" s="1"/>
       <c r="X320" s="1"/>
     </row>
-    <row r="321" spans="22:24" x14ac:dyDescent="0.25">
+    <row r="321" spans="22:24" x14ac:dyDescent="0.2">
       <c r="V321" s="1"/>
       <c r="W321" s="1"/>
       <c r="X321" s="1"/>
@@ -8298,11 +8489,11 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="187" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="M68" sqref="M68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Consultado faixa etária e leads
</commit_message>
<xml_diff>
--- a/Exercicios/Projeto02_Perfil_Dos_Clientes.xlsx
+++ b/Exercicios/Projeto02_Perfil_Dos_Clientes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guilhermefogolin/Projetos/Estudos-SQL/Exercicios/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB41DF81-AD16-754C-80E0-D6859B85B712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEFF4B0A-EDAE-CF4F-A53C-2FA851437CF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,18 +41,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
   <si>
     <t>visitas (#)</t>
   </si>
   <si>
-    <t>status profissional</t>
-  </si>
-  <si>
     <t>faixa salarial</t>
-  </si>
-  <si>
-    <t>faixa etária</t>
   </si>
   <si>
     <t>ordem</t>
@@ -110,6 +104,54 @@
   </si>
   <si>
     <t>Leads (#)</t>
+  </si>
+  <si>
+    <t>Status profissional</t>
+  </si>
+  <si>
+    <t>Leads (%)</t>
+  </si>
+  <si>
+    <t>estudante</t>
+  </si>
+  <si>
+    <t>funcionário(o) público(a)</t>
+  </si>
+  <si>
+    <t>aposentado(a)</t>
+  </si>
+  <si>
+    <t>freelancer</t>
+  </si>
+  <si>
+    <t>autônomo(a)</t>
+  </si>
+  <si>
+    <t>empresário(a)</t>
+  </si>
+  <si>
+    <t>outro</t>
+  </si>
+  <si>
+    <t>clt</t>
+  </si>
+  <si>
+    <t>Faixa etária</t>
+  </si>
+  <si>
+    <t>80+</t>
+  </si>
+  <si>
+    <t>60-80</t>
+  </si>
+  <si>
+    <t>40-60</t>
+  </si>
+  <si>
+    <t>20-40</t>
+  </si>
+  <si>
+    <t>0-20</t>
   </si>
 </sst>
 </file>
@@ -190,7 +232,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -212,6 +254,9 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -219,6 +264,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -655,7 +709,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>leads (%)</c:v>
+                  <c:v>Leads (%)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -731,13 +785,36 @@
             </c:extLst>
           </c:dLbls>
           <c:cat>
-            <c:numRef>
+            <c:strRef>
               <c:f>Output!$E$4:$E$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
+              <c:strCache>
                 <c:ptCount val="8"/>
-              </c:numCache>
-            </c:numRef>
+                <c:pt idx="0">
+                  <c:v>estudante</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>funcionário(o) público(a)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>aposentado(a)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>freelancer</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>autônomo(a)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>empresário(a)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>outro</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>clt</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -745,6 +822,30 @@
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="8"/>
+                <c:pt idx="0" formatCode="0.00%">
+                  <c:v>3.9826357083117599E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.7085507188657399E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.2614202078935799E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.2889402206380103E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.2045879963359705E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.5431120315424705E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.0445656935759997E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.64944840495439804</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -839,7 +940,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1013,7 +1114,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>leads (%)</c:v>
+                  <c:v>Leads (%)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1092,13 +1193,27 @@
             </c:extLst>
           </c:dLbls>
           <c:cat>
-            <c:numRef>
+            <c:strRef>
               <c:f>Output!$H$4:$H$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
+              <c:strCache>
                 <c:ptCount val="5"/>
-              </c:numCache>
-            </c:numRef>
+                <c:pt idx="0">
+                  <c:v>80+</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60-80</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40-60</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20-40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0-20</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -1106,6 +1221,21 @@
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2.9551156955673199E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.20279581026723401</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.32848779322155403</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.43916523955553699</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5203,8 +5333,8 @@
       <xdr:rowOff>4175</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>605114</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>18143</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>80375</xdr:rowOff>
     </xdr:to>
@@ -5731,9 +5861,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>32218</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:colOff>129038</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>101872</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -5748,8 +5878,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4658565" y="314325"/>
-          <a:ext cx="3845300" cy="3419475"/>
+          <a:off x="5129212" y="313985"/>
+          <a:ext cx="4412767" cy="4732058"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5811,6 +5941,227 @@
           </a:r>
         </a:p>
         <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" b="1">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>SELECT</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>	CASE</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>		WHEN c.professional_status = 'freelancer' THEN 'freelancer'</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>		WHEN c.professional_status = 'retired' THEN 'aposentado(a)'</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>		WHEN c.professional_status = 'clt' THEN 'clt'</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>		WHEN c.professional_status = 'self_employed' THEN 'autônomo(a)'</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>		WHEN c.professional_status = 'other' THEN 'outro'</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>		WHEN c.professional_status = 'businessman' THEN 'empresário(a)'</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>		WHEN c.professional_status = 'civil_servant' THEN 'funcionário(o) público(a)'</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>		WHEN c.professional_status = 'student' THEN 'estudante'</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>		END AS "Status profissional",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>	(COUNT(*)::float) / (SELECT COUNT(*) FROM sales.customers) AS "Leads (%)"</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>FROM sales.customers c</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>GROUP BY professional_status</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>ORDER BY "Leads (%)";</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
           <a:endParaRPr lang="en-US" sz="1100" b="0">
             <a:solidFill>
               <a:schemeClr val="dk1"/>
@@ -5835,8 +6186,8 @@
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>469247</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>101871</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -5851,8 +6202,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8726300" y="314325"/>
-          <a:ext cx="3845300" cy="3419475"/>
+          <a:off x="9667594" y="313985"/>
+          <a:ext cx="4248712" cy="3591095"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5911,6 +6262,185 @@
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
             <a:t>-- Colunas: faixa etária, leads (%)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" b="1">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>SELECT</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>	CASE</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>		WHEN datediff('y', birth_date, CURRENT_DATE) &lt; 20 THEN '0-20'</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>		WHEN datediff('y', birth_date, CURRENT_DATE) &lt; 40 THEN '20-40'</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>		WHEN datediff('y', birth_date, CURRENT_DATE) &lt; 60 THEN '40-60'</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>		WHEN datediff('y', birth_date, CURRENT_DATE) &lt; 80 THEN '60-80'</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>		ELSE '80+'</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>		END AS "Faixa etária",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>	COUNT(*)::float / (SELECT COUNT(*) FROM sales.customers) AS "Leads (%)"</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>FROM sales.customers</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>GROUP BY "Faixa etária"</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>ORDER BY "Faixa etária" DESC</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -6151,15 +6681,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>427544</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>110218</xdr:rowOff>
+      <xdr:colOff>427545</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>35511</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>29818</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>100693</xdr:rowOff>
+      <xdr:colOff>29819</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>25986</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -6174,8 +6704,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4713794" y="3920218"/>
-          <a:ext cx="3888524" cy="3419475"/>
+          <a:off x="5134016" y="5169843"/>
+          <a:ext cx="4308744" cy="3413362"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6254,15 +6784,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>277865</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>110218</xdr:rowOff>
+      <xdr:colOff>257490</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>49096</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>492460</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>100693</xdr:rowOff>
+      <xdr:colOff>472085</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>39570</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -6277,8 +6807,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8850365" y="3920218"/>
-          <a:ext cx="3888524" cy="3419475"/>
+          <a:off x="9670431" y="4042465"/>
+          <a:ext cx="4248713" cy="3413362"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6670,7 +7200,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="L32" sqref="L32"/>
+      <selection activeCell="L35" sqref="L35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6691,7 +7221,7 @@
   <dimension ref="B2:X321"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="183" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="H3" sqref="H3:I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6711,76 +7241,76 @@
   <sheetData>
     <row r="2" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="K2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="O2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="R2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="9" t="s">
+      <c r="V2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="R2" s="9" t="s">
-        <v>14</v>
+    </row>
+    <row r="3" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B3" s="13" t="s">
+        <v>19</v>
       </c>
-      <c r="V2" s="9" t="s">
-        <v>15</v>
+      <c r="C3" s="14" t="s">
+        <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B3" s="12" t="s">
+      <c r="E3" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="F3" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>1</v>
+      <c r="H3" s="14" t="s">
+        <v>31</v>
       </c>
-      <c r="F3" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>16</v>
+      <c r="I3" s="16" t="s">
+        <v>22</v>
       </c>
       <c r="J3"/>
       <c r="K3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="O3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="M3" s="1" t="s">
-        <v>4</v>
+      <c r="T3" s="1" t="s">
+        <v>2</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="V3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="W3" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="W3" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="X3" s="1" t="s">
         <v>0</v>
@@ -6788,15 +7318,23 @@
     </row>
     <row r="4" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B4" s="10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="12">
         <v>15106</v>
       </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="6"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="6"/>
+      <c r="E4" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="17">
+        <v>3.9826357083117599E-5</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" s="15">
+        <v>2.9551156955673199E-2</v>
+      </c>
       <c r="J4"/>
       <c r="K4" s="1"/>
       <c r="L4" s="6"/>
@@ -6812,15 +7350,23 @@
     </row>
     <row r="5" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B5" s="10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="12">
         <v>10003</v>
       </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="6"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="6"/>
+      <c r="E5" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="15">
+        <v>1.7085507188657399E-2</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" s="15">
+        <v>0.20279581026723401</v>
+      </c>
       <c r="J5"/>
       <c r="K5" s="1"/>
       <c r="L5" s="6"/>
@@ -6835,10 +7381,18 @@
       <c r="X5" s="1"/>
     </row>
     <row r="6" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="E6" s="1"/>
-      <c r="F6" s="6"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="6"/>
+      <c r="E6" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="15">
+        <v>4.2614202078935799E-2</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="I6" s="15">
+        <v>0.32848779322155403</v>
+      </c>
       <c r="J6"/>
       <c r="K6" s="1"/>
       <c r="L6" s="6"/>
@@ -6851,10 +7405,18 @@
       <c r="X6" s="1"/>
     </row>
     <row r="7" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="E7" s="1"/>
-      <c r="F7" s="6"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="6"/>
+      <c r="E7" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="15">
+        <v>5.2889402206380103E-2</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="I7" s="15">
+        <v>0.43916523955553699</v>
+      </c>
       <c r="J7"/>
       <c r="K7" s="1"/>
       <c r="L7" s="6"/>
@@ -6867,10 +7429,18 @@
       <c r="X7" s="1"/>
     </row>
     <row r="8" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="E8" s="1"/>
-      <c r="F8" s="6"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="6"/>
+      <c r="E8" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="15">
+        <v>7.2045879963359705E-2</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="I8" s="15">
+        <v>0</v>
+      </c>
       <c r="J8"/>
       <c r="K8" s="1"/>
       <c r="L8" s="6"/>
@@ -6883,8 +7453,12 @@
       <c r="X8" s="1"/>
     </row>
     <row r="9" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="E9" s="1"/>
-      <c r="F9" s="6"/>
+      <c r="E9" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="15">
+        <v>7.5431120315424705E-2</v>
+      </c>
       <c r="J9"/>
       <c r="R9" s="1"/>
       <c r="S9" s="2"/>
@@ -6894,16 +7468,24 @@
       <c r="X9" s="1"/>
     </row>
     <row r="10" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="E10" s="1"/>
-      <c r="F10" s="6"/>
+      <c r="E10" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="15">
+        <v>9.0445656935759997E-2</v>
+      </c>
       <c r="J10"/>
       <c r="V10" s="1"/>
       <c r="W10" s="1"/>
       <c r="X10" s="1"/>
     </row>
     <row r="11" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="E11" s="1"/>
-      <c r="F11" s="6"/>
+      <c r="E11" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="15">
+        <v>0.64944840495439804</v>
+      </c>
       <c r="J11"/>
       <c r="V11" s="1"/>
       <c r="W11" s="1"/>
@@ -8489,8 +9071,8 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="187" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M68" sqref="M68"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D12" zoomScale="187" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Consultando faixa salarial, leads e ordenação
</commit_message>
<xml_diff>
--- a/Exercicios/Projeto02_Perfil_Dos_Clientes.xlsx
+++ b/Exercicios/Projeto02_Perfil_Dos_Clientes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guilhermefogolin/Projetos/Estudos-SQL/Exercicios/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEFF4B0A-EDAE-CF4F-A53C-2FA851437CF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1146DC8A-37D9-674F-9713-9E72FA89D5EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,12 +41,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
   <si>
     <t>visitas (#)</t>
-  </si>
-  <si>
-    <t>faixa salarial</t>
   </si>
   <si>
     <t>ordem</t>
@@ -83,9 +80,6 @@
   </si>
   <si>
     <t>7-Veículos mais visitados por marca</t>
-  </si>
-  <si>
-    <t>leads (%)</t>
   </si>
   <si>
     <t>idade do veículo</t>
@@ -152,6 +146,27 @@
   </si>
   <si>
     <t>0-20</t>
+  </si>
+  <si>
+    <t>Faixa salarial</t>
+  </si>
+  <si>
+    <t>5000-10000</t>
+  </si>
+  <si>
+    <t>20000+</t>
+  </si>
+  <si>
+    <t>15000-20000</t>
+  </si>
+  <si>
+    <t>10000-15000</t>
+  </si>
+  <si>
+    <t>0-5000</t>
+  </si>
+  <si>
+    <t>Ordem</t>
   </si>
 </sst>
 </file>
@@ -232,7 +247,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -243,7 +258,6 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1485,7 +1499,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>leads (%)</c:v>
+                  <c:v>Leads (%)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1564,13 +1578,27 @@
             </c:extLst>
           </c:dLbls>
           <c:cat>
-            <c:numRef>
+            <c:strRef>
               <c:f>Output!$K$4:$K$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
+              <c:strCache>
                 <c:ptCount val="5"/>
-              </c:numCache>
-            </c:numRef>
+                <c:pt idx="0">
+                  <c:v>20000+</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15000-20000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000-15000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5000-10000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0-5000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -1578,6 +1606,21 @@
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1.6010195547413199E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.7722728901987301E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.5384125214066598E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.71026325222031905</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.16061969811621299</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -6468,8 +6511,8 @@
     <xdr:to>
       <xdr:col>27</xdr:col>
       <xdr:colOff>233924</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>169786</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -6484,8 +6527,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12726800" y="314325"/>
-          <a:ext cx="3845300" cy="3419475"/>
+          <a:off x="14138741" y="313985"/>
+          <a:ext cx="4248712" cy="4609812"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6544,6 +6587,283 @@
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
             <a:t>-- Colunas: faixa salarial, leads (%), ordem</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" b="1">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>SELECT</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>	CASE</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>		WHEN income &lt; 5000 THEN '0-5000'</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>		WHEN income &lt; 10000 THEN '5000-10000'</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>		WHEN income &lt; 15000 THEN '10000-15000'</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>		WHEN income &lt; 20000 THEN '15000-20000'</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>		ELSE '20000+'</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>		END AS "Faixa salarial",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>	COUNT(*)::float / (SELECT COUNT(*) FROM sales.customers) AS "Leads (%)",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>		CASE</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>		WHEN income &lt; 5000 THEN 1</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>		WHEN income &lt; 10000 THEN 2</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>		WHEN income &lt; 15000 THEN 3</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>		WHEN income &lt; 20000 THEN 4</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>		ELSE 5</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>		END AS "Ordem"</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>FROM sales.customers</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>GROUP BY "Faixa salarial", "Ordem"</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>ORDER BY "Ordem" DESC</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -7199,7 +7519,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="B1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="L35" sqref="L35"/>
     </sheetView>
   </sheetViews>
@@ -7220,8 +7540,8 @@
   </sheetPr>
   <dimension ref="B2:X321"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="183" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3:I3"/>
+    <sheetView showGridLines="0" topLeftCell="E1" zoomScale="183" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7240,105 +7560,111 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="H2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="K2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="O2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="O2" s="9" t="s">
+      <c r="R2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="R2" s="9" t="s">
+      <c r="V2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="V2" s="9" t="s">
+    </row>
+    <row r="3" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B3" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3"/>
+      <c r="K3" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="L3" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="R3" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B3" s="13" t="s">
-        <v>19</v>
+      <c r="S3" s="1" t="s">
+        <v>14</v>
       </c>
-      <c r="C3" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="I3" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="J3"/>
-      <c r="K3" s="1" t="s">
+      <c r="T3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L3" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="P3" s="1" t="s">
+      <c r="V3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="R3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="V3" s="1" t="s">
+      <c r="W3" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="W3" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="X3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B4" s="10" t="s">
-        <v>17</v>
+      <c r="B4" s="9" t="s">
+        <v>15</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="11">
         <v>15106</v>
       </c>
-      <c r="E4" s="11" t="s">
-        <v>23</v>
+      <c r="E4" s="10" t="s">
+        <v>21</v>
       </c>
-      <c r="F4" s="17">
+      <c r="F4" s="16">
         <v>3.9826357083117599E-5</v>
       </c>
-      <c r="H4" s="11" t="s">
-        <v>32</v>
+      <c r="H4" s="10" t="s">
+        <v>30</v>
       </c>
-      <c r="I4" s="15">
+      <c r="I4" s="14">
         <v>2.9551156955673199E-2</v>
       </c>
       <c r="J4"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="1"/>
+      <c r="K4" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="L4" s="14">
+        <v>1.6010195547413199E-2</v>
+      </c>
+      <c r="M4" s="10">
+        <v>5</v>
+      </c>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
       <c r="R4" s="1"/>
@@ -7349,28 +7675,34 @@
       <c r="X4" s="1"/>
     </row>
     <row r="5" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B5" s="10" t="s">
-        <v>18</v>
+      <c r="B5" s="9" t="s">
+        <v>16</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="11">
         <v>10003</v>
       </c>
-      <c r="E5" s="11" t="s">
-        <v>24</v>
+      <c r="E5" s="10" t="s">
+        <v>22</v>
       </c>
-      <c r="F5" s="15">
+      <c r="F5" s="14">
         <v>1.7085507188657399E-2</v>
       </c>
-      <c r="H5" s="11" t="s">
-        <v>33</v>
+      <c r="H5" s="10" t="s">
+        <v>31</v>
       </c>
-      <c r="I5" s="15">
+      <c r="I5" s="14">
         <v>0.20279581026723401</v>
       </c>
       <c r="J5"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="1"/>
+      <c r="K5" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="L5" s="14">
+        <v>1.7722728901987301E-2</v>
+      </c>
+      <c r="M5" s="10">
+        <v>4</v>
+      </c>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
       <c r="R5" s="1"/>
@@ -7381,22 +7713,28 @@
       <c r="X5" s="1"/>
     </row>
     <row r="6" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="E6" s="11" t="s">
-        <v>25</v>
+      <c r="E6" s="10" t="s">
+        <v>23</v>
       </c>
-      <c r="F6" s="15">
+      <c r="F6" s="14">
         <v>4.2614202078935799E-2</v>
       </c>
-      <c r="H6" s="11" t="s">
-        <v>34</v>
+      <c r="H6" s="10" t="s">
+        <v>32</v>
       </c>
-      <c r="I6" s="15">
+      <c r="I6" s="14">
         <v>0.32848779322155403</v>
       </c>
       <c r="J6"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="1"/>
+      <c r="K6" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="L6" s="14">
+        <v>9.5384125214066598E-2</v>
+      </c>
+      <c r="M6" s="10">
+        <v>3</v>
+      </c>
       <c r="R6" s="1"/>
       <c r="S6" s="2"/>
       <c r="T6" s="1"/>
@@ -7405,22 +7743,28 @@
       <c r="X6" s="1"/>
     </row>
     <row r="7" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="E7" s="11" t="s">
-        <v>26</v>
+      <c r="E7" s="10" t="s">
+        <v>24</v>
       </c>
-      <c r="F7" s="15">
+      <c r="F7" s="14">
         <v>5.2889402206380103E-2</v>
       </c>
-      <c r="H7" s="11" t="s">
-        <v>35</v>
+      <c r="H7" s="10" t="s">
+        <v>33</v>
       </c>
-      <c r="I7" s="15">
+      <c r="I7" s="14">
         <v>0.43916523955553699</v>
       </c>
       <c r="J7"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="1"/>
+      <c r="K7" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="L7" s="14">
+        <v>0.71026325222031905</v>
+      </c>
+      <c r="M7" s="10">
+        <v>2</v>
+      </c>
       <c r="R7" s="1"/>
       <c r="S7" s="2"/>
       <c r="T7" s="1"/>
@@ -7429,22 +7773,28 @@
       <c r="X7" s="1"/>
     </row>
     <row r="8" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="E8" s="11" t="s">
-        <v>27</v>
+      <c r="E8" s="10" t="s">
+        <v>25</v>
       </c>
-      <c r="F8" s="15">
+      <c r="F8" s="14">
         <v>7.2045879963359705E-2</v>
       </c>
-      <c r="H8" s="11" t="s">
-        <v>36</v>
+      <c r="H8" s="10" t="s">
+        <v>34</v>
       </c>
-      <c r="I8" s="15">
+      <c r="I8" s="14">
         <v>0</v>
       </c>
       <c r="J8"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="1"/>
+      <c r="K8" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="L8" s="14">
+        <v>0.16061969811621299</v>
+      </c>
+      <c r="M8" s="10">
+        <v>1</v>
+      </c>
       <c r="R8" s="1"/>
       <c r="S8" s="2"/>
       <c r="T8" s="1"/>
@@ -7453,10 +7803,10 @@
       <c r="X8" s="1"/>
     </row>
     <row r="9" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="E9" s="11" t="s">
-        <v>28</v>
+      <c r="E9" s="10" t="s">
+        <v>26</v>
       </c>
-      <c r="F9" s="15">
+      <c r="F9" s="14">
         <v>7.5431120315424705E-2</v>
       </c>
       <c r="J9"/>
@@ -7468,10 +7818,10 @@
       <c r="X9" s="1"/>
     </row>
     <row r="10" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="E10" s="11" t="s">
-        <v>29</v>
+      <c r="E10" s="10" t="s">
+        <v>27</v>
       </c>
-      <c r="F10" s="15">
+      <c r="F10" s="14">
         <v>9.0445656935759997E-2</v>
       </c>
       <c r="J10"/>
@@ -7480,10 +7830,10 @@
       <c r="X10" s="1"/>
     </row>
     <row r="11" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="E11" s="11" t="s">
-        <v>30</v>
+      <c r="E11" s="10" t="s">
+        <v>28</v>
       </c>
-      <c r="F11" s="15">
+      <c r="F11" s="14">
         <v>0.64944840495439804</v>
       </c>
       <c r="J11"/>
@@ -7582,7 +7932,7 @@
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
       <c r="I29" s="4"/>
-      <c r="J29" s="7"/>
+      <c r="J29" s="6"/>
       <c r="K29" s="4"/>
       <c r="L29" s="4"/>
       <c r="M29" s="4"/>
@@ -7595,7 +7945,7 @@
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
-      <c r="J30" s="8"/>
+      <c r="J30" s="7"/>
       <c r="K30" s="5"/>
       <c r="L30" s="5"/>
       <c r="M30" s="5"/>
@@ -9071,7 +9421,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D12" zoomScale="187" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A17" zoomScale="187" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Consultando classificação dos veículos
</commit_message>
<xml_diff>
--- a/Exercicios/Projeto02_Perfil_Dos_Clientes.xlsx
+++ b/Exercicios/Projeto02_Perfil_Dos_Clientes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guilhermefogolin/Projetos/Estudos-SQL/Exercicios/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1146DC8A-37D9-674F-9713-9E72FA89D5EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED346867-8927-4142-8656-841D9B7931FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,18 +41,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
   <si>
     <t>visitas (#)</t>
   </si>
   <si>
     <t>ordem</t>
-  </si>
-  <si>
-    <t>classificação do veículo</t>
-  </si>
-  <si>
-    <t>veículos visitados (#)</t>
   </si>
   <si>
     <t>brand</t>
@@ -167,6 +161,18 @@
   </si>
   <si>
     <t>Ordem</t>
+  </si>
+  <si>
+    <t>Classificação</t>
+  </si>
+  <si>
+    <t>Veículos visitados</t>
+  </si>
+  <si>
+    <t>Seminovo</t>
+  </si>
+  <si>
+    <t>Novo</t>
   </si>
 </sst>
 </file>
@@ -1878,7 +1884,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>veículos visitados (#)</c:v>
+                  <c:v>Veículos visitados</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1989,13 +1995,18 @@
             </c:extLst>
           </c:dLbls>
           <c:cat>
-            <c:numRef>
+            <c:strRef>
               <c:f>Output!$O$4:$O$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
+              <c:strCache>
                 <c:ptCount val="2"/>
-              </c:numCache>
-            </c:numRef>
+                <c:pt idx="0">
+                  <c:v>Seminovo</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Novo</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -2003,6 +2014,12 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>29418</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1162</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -6891,8 +6908,8 @@
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>193104</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>100693</xdr:rowOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>13511</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -6907,8 +6924,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="590830" y="3920218"/>
-          <a:ext cx="3888524" cy="3419475"/>
+          <a:off x="590830" y="3893197"/>
+          <a:ext cx="4330997" cy="4632016"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6981,6 +6998,280 @@
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
             <a:t>-- Regra de negócio: Veículos novos tem até 2 anos e seminovos acima de 2 anos</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" b="1">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>WITH classificacao AS (</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>	SELECT</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>		f.visit_page_date,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>		p.model_year,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>		EXTRACT('y' FROM visit_page_date) - p.model_year::int AS idade,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>		CASE</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>			WHEN (EXTRACT('y' FROM visit_page_date) - p.model_year::int) &lt;= 2 THEN 'Novo'</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>			ELSE 'Seminovo'</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>			END AS "Classificação"</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>	FROM sales.funnel f</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>	LEFT JOIN sales.products p</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>	ON f.product_id = p.product_id</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" b="1">
+            <a:solidFill>
+              <a:srgbClr val="00B050"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>SELECT</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>	"Classificação",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>	COUNT(*) AS "Veículos visitados"</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>FROM classificacao</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>GROUP BY "Classificação";</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -7540,8 +7831,8 @@
   </sheetPr>
   <dimension ref="B2:X321"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="E1" zoomScale="183" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView showGridLines="0" topLeftCell="J1" zoomScale="183" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7561,76 +7852,76 @@
   <sheetData>
     <row r="2" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="K2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="O2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="R2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="O2" s="8" t="s">
+      <c r="V2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="R2" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="V2" s="8" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="3" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B3" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="F3" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" s="15" t="s">
-        <v>20</v>
-      </c>
       <c r="H3" s="13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J3"/>
       <c r="K3" s="13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="L3" s="15" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="M3" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="O3" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="P3" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="O3" s="1" t="s">
-        <v>2</v>
+      <c r="R3" s="13" t="s">
+        <v>11</v>
       </c>
-      <c r="P3" s="1" t="s">
-        <v>3</v>
+      <c r="S3" s="15" t="s">
+        <v>12</v>
       </c>
-      <c r="R3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="T3" s="1" t="s">
+      <c r="T3" s="13" t="s">
         <v>1</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="W3" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="X3" s="1" t="s">
         <v>0</v>
@@ -7638,26 +7929,26 @@
     </row>
     <row r="4" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B4" s="9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C4" s="11">
         <v>15106</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F4" s="16">
         <v>3.9826357083117599E-5</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I4" s="14">
         <v>2.9551156955673199E-2</v>
       </c>
       <c r="J4"/>
       <c r="K4" s="10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="L4" s="14">
         <v>1.6010195547413199E-2</v>
@@ -7665,37 +7956,41 @@
       <c r="M4" s="10">
         <v>5</v>
       </c>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="R4" s="1"/>
-      <c r="S4" s="2"/>
-      <c r="T4" s="1"/>
+      <c r="O4" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="P4" s="10">
+        <v>29418</v>
+      </c>
+      <c r="R4" s="10"/>
+      <c r="S4" s="14"/>
+      <c r="T4" s="10"/>
       <c r="V4" s="1"/>
       <c r="W4" s="1"/>
       <c r="X4" s="1"/>
     </row>
     <row r="5" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B5" s="9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C5" s="11">
         <v>10003</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F5" s="14">
         <v>1.7085507188657399E-2</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I5" s="14">
         <v>0.20279581026723401</v>
       </c>
       <c r="J5"/>
       <c r="K5" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="L5" s="14">
         <v>1.7722728901987301E-2</v>
@@ -7703,31 +7998,35 @@
       <c r="M5" s="10">
         <v>4</v>
       </c>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
-      <c r="R5" s="1"/>
-      <c r="S5" s="2"/>
-      <c r="T5" s="1"/>
+      <c r="O5" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="P5" s="10">
+        <v>1162</v>
+      </c>
+      <c r="R5" s="10"/>
+      <c r="S5" s="14"/>
+      <c r="T5" s="10"/>
       <c r="V5" s="1"/>
       <c r="W5" s="1"/>
       <c r="X5" s="1"/>
     </row>
     <row r="6" spans="2:24" x14ac:dyDescent="0.2">
       <c r="E6" s="10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F6" s="14">
         <v>4.2614202078935799E-2</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I6" s="14">
         <v>0.32848779322155403</v>
       </c>
       <c r="J6"/>
       <c r="K6" s="10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="L6" s="14">
         <v>9.5384125214066598E-2</v>
@@ -7735,29 +8034,29 @@
       <c r="M6" s="10">
         <v>3</v>
       </c>
-      <c r="R6" s="1"/>
-      <c r="S6" s="2"/>
-      <c r="T6" s="1"/>
+      <c r="R6" s="10"/>
+      <c r="S6" s="14"/>
+      <c r="T6" s="10"/>
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
       <c r="X6" s="1"/>
     </row>
     <row r="7" spans="2:24" x14ac:dyDescent="0.2">
       <c r="E7" s="10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F7" s="14">
         <v>5.2889402206380103E-2</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I7" s="14">
         <v>0.43916523955553699</v>
       </c>
       <c r="J7"/>
       <c r="K7" s="10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="L7" s="14">
         <v>0.71026325222031905</v>
@@ -7765,29 +8064,29 @@
       <c r="M7" s="10">
         <v>2</v>
       </c>
-      <c r="R7" s="1"/>
-      <c r="S7" s="2"/>
-      <c r="T7" s="1"/>
+      <c r="R7" s="10"/>
+      <c r="S7" s="14"/>
+      <c r="T7" s="10"/>
       <c r="V7" s="1"/>
       <c r="W7" s="1"/>
       <c r="X7" s="1"/>
     </row>
     <row r="8" spans="2:24" x14ac:dyDescent="0.2">
       <c r="E8" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F8" s="14">
         <v>7.2045879963359705E-2</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I8" s="14">
         <v>0</v>
       </c>
       <c r="J8"/>
       <c r="K8" s="10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="L8" s="14">
         <v>0.16061969811621299</v>
@@ -7795,16 +8094,16 @@
       <c r="M8" s="10">
         <v>1</v>
       </c>
-      <c r="R8" s="1"/>
-      <c r="S8" s="2"/>
-      <c r="T8" s="1"/>
+      <c r="R8" s="10"/>
+      <c r="S8" s="14"/>
+      <c r="T8" s="10"/>
       <c r="V8" s="1"/>
       <c r="W8" s="1"/>
       <c r="X8" s="1"/>
     </row>
     <row r="9" spans="2:24" x14ac:dyDescent="0.2">
       <c r="E9" s="10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F9" s="14">
         <v>7.5431120315424705E-2</v>
@@ -7819,7 +8118,7 @@
     </row>
     <row r="10" spans="2:24" x14ac:dyDescent="0.2">
       <c r="E10" s="10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F10" s="14">
         <v>9.0445656935759997E-2</v>
@@ -7831,7 +8130,7 @@
     </row>
     <row r="11" spans="2:24" x14ac:dyDescent="0.2">
       <c r="E11" s="10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F11" s="14">
         <v>0.64944840495439804</v>
@@ -9421,7 +9720,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A17" zoomScale="187" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="94" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Consultando idade dos veículos
</commit_message>
<xml_diff>
--- a/Exercicios/Projeto02_Perfil_Dos_Clientes.xlsx
+++ b/Exercicios/Projeto02_Perfil_Dos_Clientes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guilhermefogolin/Projetos/Estudos-SQL/Exercicios/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED346867-8927-4142-8656-841D9B7931FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A09EB15E-206B-EE4F-A6EC-DEF2A406C06D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,12 +41,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="49">
   <si>
     <t>visitas (#)</t>
-  </si>
-  <si>
-    <t>ordem</t>
   </si>
   <si>
     <t>brand</t>
@@ -74,12 +71,6 @@
   </si>
   <si>
     <t>7-Veículos mais visitados por marca</t>
-  </si>
-  <si>
-    <t>idade do veículo</t>
-  </si>
-  <si>
-    <t>veículos visitados (%)</t>
   </si>
   <si>
     <t>Mulheres</t>
@@ -173,6 +164,30 @@
   </si>
   <si>
     <t>Novo</t>
+  </si>
+  <si>
+    <t>Idade do veículo</t>
+  </si>
+  <si>
+    <t>Veículos visitados (%)</t>
+  </si>
+  <si>
+    <t>Até 2 anos</t>
+  </si>
+  <si>
+    <t>Até 2 à 4 anos</t>
+  </si>
+  <si>
+    <t>Até 4 à 6 anos</t>
+  </si>
+  <si>
+    <t>Até 6 à 8 anos</t>
+  </si>
+  <si>
+    <t>Até 8 à 10 anos</t>
+  </si>
+  <si>
+    <t>Acima de 10 anos</t>
   </si>
 </sst>
 </file>
@@ -2191,7 +2206,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>veículos visitados (%)</c:v>
+                  <c:v>Veículos visitados (%)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2267,13 +2282,30 @@
             </c:extLst>
           </c:dLbls>
           <c:cat>
-            <c:numRef>
+            <c:strRef>
               <c:f>Output!$R$4:$R$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
+              <c:strCache>
                 <c:ptCount val="6"/>
-              </c:numCache>
-            </c:numRef>
+                <c:pt idx="0">
+                  <c:v>Até 2 anos</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Até 2 à 4 anos</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Até 4 à 6 anos</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Até 6 à 8 anos</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Até 8 à 10 anos</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Acima de 10 anos</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -2281,6 +2313,24 @@
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3.7998691955526402E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.10775016350555899</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.18103335513407401</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.19630477436232799</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.24767822105951601</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.22923479398299501</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -7299,8 +7349,8 @@
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>29819</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>25986</xdr:rowOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>65689</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -7315,8 +7365,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5134016" y="5169843"/>
-          <a:ext cx="4308744" cy="3413362"/>
+          <a:off x="5102459" y="5060770"/>
+          <a:ext cx="4277188" cy="8963971"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7375,6 +7425,476 @@
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
             <a:t>-- Colunas: Idade do veículo, veículos visitados (%), ordem</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" b="1">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>WITH faixa_idade AS (</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>	SELECT</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>		f.visit_page_date,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>		p.model_year,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>		EXTRACT('y' FROM visit_page_date) - p.model_year::int AS idade,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>		CASE</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>			WHEN (EXTRACT('y' FROM visit_page_date) - p.model_year::int) &lt;= 2 THEN 'Até 2 anos'</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>			WHEN (EXTRACT('y' FROM visit_page_date) - p.model_year::int) &lt;= 4 THEN 'Até 2 à 4 anos'</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>			WHEN (EXTRACT('y' FROM visit_page_date) - p.model_year::int) &lt;= 6 THEN 'Até 4 à 6 anos'</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>			WHEN (EXTRACT('y' FROM visit_page_date) - p.model_year::int) &lt;= 8 THEN 'Até 6 à 8 anos'</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>			WHEN (EXTRACT('y' FROM visit_page_date) - p.model_year::int) &lt;= 10 THEN 'Até 8 à 10 anos'</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>			ELSE 'Acima de 10 anos'</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>			END AS "Idade do veículo",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>		CASE</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>			WHEN (EXTRACT('y' FROM visit_page_date) - p.model_year::int) &lt;= 2 THEN 1</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>			WHEN (EXTRACT('y' FROM visit_page_date) - p.model_year::int) &lt;= 4 THEN 2</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>			WHEN (EXTRACT('y' FROM visit_page_date) - p.model_year::int) &lt;= 6 THEN 3</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>			WHEN (EXTRACT('y' FROM visit_page_date) - p.model_year::int) &lt;= 8 THEN 4</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>			WHEN (EXTRACT('y' FROM visit_page_date) - p.model_year::int) &lt;= 10 THEN 5</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>			ELSE 6</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>			END AS "Ordem"</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>	FROM sales.funnel f</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>	LEFT JOIN sales.products p</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>	ON f.product_id = p.product_id</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" b="1">
+            <a:solidFill>
+              <a:srgbClr val="00B050"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>SELECT</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>	"Idade do veículo",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>	COUNT(*)::float / (SELECT COUNT(*) FROM sales.funnel) AS "Veículos visitados (%)",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>	"Ordem"</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>FROM faixa_idade</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>GROUP BY "Idade do veículo", "Ordem"</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>ORDER BY "Ordem";</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -7832,7 +8352,7 @@
   <dimension ref="B2:X321"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="J1" zoomScale="183" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7852,76 +8372,76 @@
   <sheetData>
     <row r="2" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B2" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="H2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="K2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="O2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="O2" s="8" t="s">
+      <c r="R2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="R2" s="8" t="s">
+      <c r="V2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="V2" s="8" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="3" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B3" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="15" t="s">
-        <v>18</v>
-      </c>
       <c r="H3" s="13" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="J3"/>
       <c r="K3" s="13" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="L3" s="15" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="M3" s="13" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="O3" s="13" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="P3" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="R3" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="R3" s="13" t="s">
-        <v>11</v>
-      </c>
       <c r="S3" s="15" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="T3" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="V3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="V3" s="1" t="s">
+      <c r="W3" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="W3" s="1" t="s">
-        <v>3</v>
       </c>
       <c r="X3" s="1" t="s">
         <v>0</v>
@@ -7929,26 +8449,26 @@
     </row>
     <row r="4" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B4" s="9" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C4" s="11">
         <v>15106</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F4" s="16">
         <v>3.9826357083117599E-5</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I4" s="14">
         <v>2.9551156955673199E-2</v>
       </c>
       <c r="J4"/>
       <c r="K4" s="10" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="L4" s="14">
         <v>1.6010195547413199E-2</v>
@@ -7957,40 +8477,46 @@
         <v>5</v>
       </c>
       <c r="O4" s="10" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="P4" s="10">
         <v>29418</v>
       </c>
-      <c r="R4" s="10"/>
-      <c r="S4" s="14"/>
-      <c r="T4" s="10"/>
+      <c r="R4" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="S4" s="14">
+        <v>3.7998691955526402E-2</v>
+      </c>
+      <c r="T4" s="10">
+        <v>1</v>
+      </c>
       <c r="V4" s="1"/>
       <c r="W4" s="1"/>
       <c r="X4" s="1"/>
     </row>
     <row r="5" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B5" s="9" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C5" s="11">
         <v>10003</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F5" s="14">
         <v>1.7085507188657399E-2</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="I5" s="14">
         <v>0.20279581026723401</v>
       </c>
       <c r="J5"/>
       <c r="K5" s="10" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="L5" s="14">
         <v>1.7722728901987301E-2</v>
@@ -7999,34 +8525,40 @@
         <v>4</v>
       </c>
       <c r="O5" s="10" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="P5" s="10">
         <v>1162</v>
       </c>
-      <c r="R5" s="10"/>
-      <c r="S5" s="14"/>
-      <c r="T5" s="10"/>
+      <c r="R5" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="S5" s="14">
+        <v>0.10775016350555899</v>
+      </c>
+      <c r="T5" s="10">
+        <v>2</v>
+      </c>
       <c r="V5" s="1"/>
       <c r="W5" s="1"/>
       <c r="X5" s="1"/>
     </row>
     <row r="6" spans="2:24" x14ac:dyDescent="0.2">
       <c r="E6" s="10" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F6" s="14">
         <v>4.2614202078935799E-2</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="I6" s="14">
         <v>0.32848779322155403</v>
       </c>
       <c r="J6"/>
       <c r="K6" s="10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="L6" s="14">
         <v>9.5384125214066598E-2</v>
@@ -8034,29 +8566,35 @@
       <c r="M6" s="10">
         <v>3</v>
       </c>
-      <c r="R6" s="10"/>
-      <c r="S6" s="14"/>
-      <c r="T6" s="10"/>
+      <c r="R6" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="S6" s="14">
+        <v>0.18103335513407401</v>
+      </c>
+      <c r="T6" s="10">
+        <v>3</v>
+      </c>
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
       <c r="X6" s="1"/>
     </row>
     <row r="7" spans="2:24" x14ac:dyDescent="0.2">
       <c r="E7" s="10" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F7" s="14">
         <v>5.2889402206380103E-2</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I7" s="14">
         <v>0.43916523955553699</v>
       </c>
       <c r="J7"/>
       <c r="K7" s="10" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="L7" s="14">
         <v>0.71026325222031905</v>
@@ -8064,29 +8602,35 @@
       <c r="M7" s="10">
         <v>2</v>
       </c>
-      <c r="R7" s="10"/>
-      <c r="S7" s="14"/>
-      <c r="T7" s="10"/>
+      <c r="R7" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="S7" s="14">
+        <v>0.19630477436232799</v>
+      </c>
+      <c r="T7" s="10">
+        <v>4</v>
+      </c>
       <c r="V7" s="1"/>
       <c r="W7" s="1"/>
       <c r="X7" s="1"/>
     </row>
     <row r="8" spans="2:24" x14ac:dyDescent="0.2">
       <c r="E8" s="10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F8" s="14">
         <v>7.2045879963359705E-2</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="I8" s="14">
         <v>0</v>
       </c>
       <c r="J8"/>
       <c r="K8" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="L8" s="14">
         <v>0.16061969811621299</v>
@@ -8094,31 +8638,43 @@
       <c r="M8" s="10">
         <v>1</v>
       </c>
-      <c r="R8" s="10"/>
-      <c r="S8" s="14"/>
-      <c r="T8" s="10"/>
+      <c r="R8" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="S8" s="14">
+        <v>0.24767822105951601</v>
+      </c>
+      <c r="T8" s="10">
+        <v>5</v>
+      </c>
       <c r="V8" s="1"/>
       <c r="W8" s="1"/>
       <c r="X8" s="1"/>
     </row>
     <row r="9" spans="2:24" x14ac:dyDescent="0.2">
       <c r="E9" s="10" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F9" s="14">
         <v>7.5431120315424705E-2</v>
       </c>
       <c r="J9"/>
-      <c r="R9" s="1"/>
-      <c r="S9" s="2"/>
-      <c r="T9" s="1"/>
+      <c r="R9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="S9" s="2">
+        <v>0.22923479398299501</v>
+      </c>
+      <c r="T9" s="1">
+        <v>6</v>
+      </c>
       <c r="V9" s="1"/>
       <c r="W9" s="1"/>
       <c r="X9" s="1"/>
     </row>
     <row r="10" spans="2:24" x14ac:dyDescent="0.2">
       <c r="E10" s="10" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F10" s="14">
         <v>9.0445656935759997E-2</v>
@@ -8130,7 +8686,7 @@
     </row>
     <row r="11" spans="2:24" x14ac:dyDescent="0.2">
       <c r="E11" s="10" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F11" s="14">
         <v>0.64944840495439804</v>
@@ -9720,8 +10276,8 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="94" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A28" zoomScale="116" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Y34" sqref="Y34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Finalizando o projeto 02
</commit_message>
<xml_diff>
--- a/Exercicios/Projeto02_Perfil_Dos_Clientes.xlsx
+++ b/Exercicios/Projeto02_Perfil_Dos_Clientes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guilhermefogolin/Projetos/Estudos-SQL/Exercicios/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5C4B91B-47CA-0741-8A9B-7CB968CD0B8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B50705F-6981-2443-9DE0-4379FDD220F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="6" r:id="rId1"/>
@@ -1273,7 +1273,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -1315,7 +1315,6 @@
     <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -9473,7 +9472,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="F1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="L35" sqref="L35"/>
     </sheetView>
   </sheetViews>
@@ -9494,8 +9493,8 @@
   </sheetPr>
   <dimension ref="B2:X321"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="J1" zoomScale="183" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="O1" zoomScale="183" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Y6" sqref="Y6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9580,13 +9579,13 @@
       <c r="T3" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="V3" s="17" t="s">
+      <c r="V3" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="W3" s="17" t="s">
+      <c r="W3" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="X3" s="17" t="s">
+      <c r="X3" s="13" t="s">
         <v>48</v>
       </c>
     </row>
@@ -9634,13 +9633,13 @@
       <c r="T4" s="10">
         <v>1</v>
       </c>
-      <c r="V4" s="1" t="s">
+      <c r="V4" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="W4" s="1" t="s">
+      <c r="W4" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="X4" s="1">
+      <c r="X4" s="10">
         <v>18</v>
       </c>
     </row>
@@ -9688,13 +9687,13 @@
       <c r="T5" s="10">
         <v>2</v>
       </c>
-      <c r="V5" s="1" t="s">
+      <c r="V5" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="W5" s="1" t="s">
+      <c r="W5" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="X5" s="1">
+      <c r="X5" s="10">
         <v>32</v>
       </c>
     </row>
@@ -9730,13 +9729,13 @@
       <c r="T6" s="10">
         <v>3</v>
       </c>
-      <c r="V6" s="1" t="s">
+      <c r="V6" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="W6" s="1" t="s">
+      <c r="W6" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="X6" s="1">
+      <c r="X6" s="10">
         <v>19</v>
       </c>
     </row>
@@ -9772,13 +9771,13 @@
       <c r="T7" s="10">
         <v>4</v>
       </c>
-      <c r="V7" s="1" t="s">
+      <c r="V7" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="W7" s="1" t="s">
+      <c r="W7" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="X7" s="1">
+      <c r="X7" s="10">
         <v>7</v>
       </c>
     </row>
@@ -9814,13 +9813,13 @@
       <c r="T8" s="10">
         <v>5</v>
       </c>
-      <c r="V8" s="1" t="s">
+      <c r="V8" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="W8" s="1" t="s">
+      <c r="W8" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="X8" s="1">
+      <c r="X8" s="10">
         <v>1</v>
       </c>
     </row>
@@ -9841,13 +9840,13 @@
       <c r="T9" s="1">
         <v>6</v>
       </c>
-      <c r="V9" s="1" t="s">
+      <c r="V9" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="W9" s="1" t="s">
+      <c r="W9" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="X9" s="1">
+      <c r="X9" s="10">
         <v>1</v>
       </c>
     </row>
@@ -9859,13 +9858,13 @@
         <v>9.0445656935759997E-2</v>
       </c>
       <c r="J10"/>
-      <c r="V10" s="1" t="s">
+      <c r="V10" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="W10" s="1" t="s">
+      <c r="W10" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="X10" s="1">
+      <c r="X10" s="10">
         <v>30</v>
       </c>
     </row>
@@ -9877,201 +9876,201 @@
         <v>0.64944840495439804</v>
       </c>
       <c r="J11"/>
-      <c r="V11" s="1" t="s">
+      <c r="V11" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="W11" s="1" t="s">
+      <c r="W11" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="X11" s="1">
+      <c r="X11" s="10">
         <v>6</v>
       </c>
     </row>
     <row r="12" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="V12" s="1" t="s">
+      <c r="V12" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="W12" s="1" t="s">
+      <c r="W12" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="X12" s="1">
+      <c r="X12" s="10">
         <v>4</v>
       </c>
     </row>
     <row r="13" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="V13" s="1" t="s">
+      <c r="V13" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="W13" s="1" t="s">
+      <c r="W13" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="X13" s="1">
+      <c r="X13" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="V14" s="1" t="s">
+      <c r="V14" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="W14" s="1" t="s">
+      <c r="W14" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="X14" s="1">
+      <c r="X14" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="V15" s="1" t="s">
+      <c r="V15" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="W15" s="1" t="s">
+      <c r="W15" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="X15" s="1">
+      <c r="X15" s="10">
         <v>4</v>
       </c>
     </row>
     <row r="16" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="V16" s="1" t="s">
+      <c r="V16" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="W16" s="1" t="s">
+      <c r="W16" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="X16" s="1">
+      <c r="X16" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="4:24" x14ac:dyDescent="0.2">
-      <c r="V17" s="1" t="s">
+      <c r="V17" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="W17" s="1">
+      <c r="W17" s="10">
         <v>0</v>
       </c>
-      <c r="X17" s="1">
+      <c r="X17" s="10">
         <v>32</v>
       </c>
     </row>
     <row r="18" spans="4:24" x14ac:dyDescent="0.2">
-      <c r="V18" s="1" t="s">
+      <c r="V18" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="W18" s="1" t="s">
+      <c r="W18" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="X18" s="1">
+      <c r="X18" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="4:24" x14ac:dyDescent="0.2">
-      <c r="V19" s="1" t="s">
+      <c r="V19" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="W19" s="1" t="s">
+      <c r="W19" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="X19" s="1">
+      <c r="X19" s="10">
         <v>13</v>
       </c>
     </row>
     <row r="20" spans="4:24" x14ac:dyDescent="0.2">
-      <c r="V20" s="1" t="s">
+      <c r="V20" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="W20" s="1" t="s">
+      <c r="W20" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="X20" s="1">
+      <c r="X20" s="10">
         <v>6</v>
       </c>
     </row>
     <row r="21" spans="4:24" x14ac:dyDescent="0.2">
-      <c r="V21" s="1" t="s">
+      <c r="V21" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="W21" s="1" t="s">
+      <c r="W21" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="X21" s="1">
+      <c r="X21" s="10">
         <v>8</v>
       </c>
     </row>
     <row r="22" spans="4:24" x14ac:dyDescent="0.2">
-      <c r="V22" s="1" t="s">
+      <c r="V22" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="W22" s="1" t="s">
+      <c r="W22" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="X22" s="1">
+      <c r="X22" s="10">
         <v>2</v>
       </c>
     </row>
     <row r="23" spans="4:24" x14ac:dyDescent="0.2">
-      <c r="V23" s="1" t="s">
+      <c r="V23" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="W23" s="1" t="s">
+      <c r="W23" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="X23" s="1">
+      <c r="X23" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="4:24" x14ac:dyDescent="0.2">
-      <c r="V24" s="1" t="s">
+      <c r="V24" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="W24" s="1" t="s">
+      <c r="W24" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="X24" s="1">
+      <c r="X24" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="4:24" x14ac:dyDescent="0.2">
-      <c r="V25" s="1" t="s">
+      <c r="V25" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="W25" s="1" t="s">
+      <c r="W25" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="X25" s="1">
+      <c r="X25" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="4:24" x14ac:dyDescent="0.2">
-      <c r="V26" s="1" t="s">
+      <c r="V26" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="W26" s="1" t="s">
+      <c r="W26" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="X26" s="1">
+      <c r="X26" s="10">
         <v>2</v>
       </c>
     </row>
     <row r="27" spans="4:24" x14ac:dyDescent="0.2">
-      <c r="V27" s="1" t="s">
+      <c r="V27" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="W27" s="1" t="s">
+      <c r="W27" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="X27" s="1">
+      <c r="X27" s="10">
         <v>7</v>
       </c>
     </row>
     <row r="28" spans="4:24" x14ac:dyDescent="0.2">
       <c r="D28" s="3"/>
-      <c r="V28" s="1" t="s">
+      <c r="V28" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="W28" s="1" t="s">
+      <c r="W28" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="X28" s="1">
+      <c r="X28" s="10">
         <v>32</v>
       </c>
     </row>
@@ -10084,13 +10083,13 @@
       <c r="K29" s="4"/>
       <c r="L29" s="4"/>
       <c r="M29" s="4"/>
-      <c r="V29" s="1" t="s">
+      <c r="V29" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="W29" s="1" t="s">
+      <c r="W29" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="X29" s="1">
+      <c r="X29" s="10">
         <v>9</v>
       </c>
     </row>
@@ -10103,3214 +10102,3214 @@
       <c r="K30" s="5"/>
       <c r="L30" s="5"/>
       <c r="M30" s="5"/>
-      <c r="V30" s="1" t="s">
+      <c r="V30" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="W30" s="1" t="s">
+      <c r="W30" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="X30" s="1">
+      <c r="X30" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="31" spans="4:24" x14ac:dyDescent="0.2">
-      <c r="V31" s="1" t="s">
+      <c r="V31" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="W31" s="1" t="s">
+      <c r="W31" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="X31" s="1">
+      <c r="X31" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="32" spans="4:24" x14ac:dyDescent="0.2">
-      <c r="V32" s="1" t="s">
+      <c r="V32" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="W32" s="1" t="s">
+      <c r="W32" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="X32" s="1">
+      <c r="X32" s="10">
         <v>2</v>
       </c>
     </row>
     <row r="33" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V33" s="1" t="s">
+      <c r="V33" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="W33" s="1" t="s">
+      <c r="W33" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="X33" s="1">
+      <c r="X33" s="10">
         <v>2</v>
       </c>
     </row>
     <row r="34" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V34" s="1" t="s">
+      <c r="V34" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="W34" s="1" t="s">
+      <c r="W34" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="X34" s="1">
+      <c r="X34" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="35" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V35" s="1" t="s">
+      <c r="V35" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="W35" s="1" t="s">
+      <c r="W35" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="X35" s="1">
+      <c r="X35" s="10">
         <v>2</v>
       </c>
     </row>
     <row r="36" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V36" s="1" t="s">
+      <c r="V36" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="W36" s="1" t="s">
+      <c r="W36" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="X36" s="1">
+      <c r="X36" s="10">
         <v>57</v>
       </c>
     </row>
     <row r="37" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V37" s="1" t="s">
+      <c r="V37" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="W37" s="1" t="s">
+      <c r="W37" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="X37" s="1">
+      <c r="X37" s="10">
         <v>6</v>
       </c>
     </row>
     <row r="38" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V38" s="1" t="s">
+      <c r="V38" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="W38" s="1" t="s">
+      <c r="W38" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="X38" s="1">
+      <c r="X38" s="10">
         <v>5</v>
       </c>
     </row>
     <row r="39" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V39" s="1" t="s">
+      <c r="V39" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="W39" s="1" t="s">
+      <c r="W39" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="X39" s="1">
+      <c r="X39" s="10">
         <v>2</v>
       </c>
     </row>
     <row r="40" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V40" s="1" t="s">
+      <c r="V40" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="W40" s="1" t="s">
+      <c r="W40" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="X40" s="1">
+      <c r="X40" s="10">
         <v>5</v>
       </c>
     </row>
     <row r="41" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V41" s="1" t="s">
+      <c r="V41" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="W41" s="1" t="s">
+      <c r="W41" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="X41" s="1">
+      <c r="X41" s="10">
         <v>19</v>
       </c>
     </row>
     <row r="42" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V42" s="1" t="s">
+      <c r="V42" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="W42" s="1" t="s">
+      <c r="W42" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="X42" s="1">
+      <c r="X42" s="10">
         <v>4</v>
       </c>
     </row>
     <row r="43" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V43" s="1" t="s">
+      <c r="V43" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="W43" s="1" t="s">
+      <c r="W43" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="X43" s="1">
+      <c r="X43" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="44" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V44" s="1" t="s">
+      <c r="V44" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="W44" s="1" t="s">
+      <c r="W44" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="X44" s="1">
+      <c r="X44" s="10">
         <v>12</v>
       </c>
     </row>
     <row r="45" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V45" s="1" t="s">
+      <c r="V45" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="W45" s="1" t="s">
+      <c r="W45" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="X45" s="1">
+      <c r="X45" s="10">
         <v>4</v>
       </c>
     </row>
     <row r="46" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V46" s="1" t="s">
+      <c r="V46" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="W46" s="1" t="s">
+      <c r="W46" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="X46" s="1">
+      <c r="X46" s="10">
         <v>11</v>
       </c>
     </row>
     <row r="47" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V47" s="1" t="s">
+      <c r="V47" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="W47" s="1" t="s">
+      <c r="W47" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="X47" s="1">
+      <c r="X47" s="10">
         <v>21</v>
       </c>
     </row>
     <row r="48" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V48" s="1" t="s">
+      <c r="V48" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="W48" s="1" t="s">
+      <c r="W48" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="X48" s="1">
+      <c r="X48" s="10">
         <v>22</v>
       </c>
     </row>
     <row r="49" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V49" s="1" t="s">
+      <c r="V49" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="W49" s="1">
+      <c r="W49" s="10">
         <v>0</v>
       </c>
-      <c r="X49" s="1">
+      <c r="X49" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="50" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V50" s="1" t="s">
+      <c r="V50" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="W50" s="1" t="s">
+      <c r="W50" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="X50" s="1">
+      <c r="X50" s="10">
         <v>249</v>
       </c>
     </row>
     <row r="51" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V51" s="1" t="s">
+      <c r="V51" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="W51" s="1" t="s">
+      <c r="W51" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="X51" s="1">
+      <c r="X51" s="10">
         <v>145</v>
       </c>
     </row>
     <row r="52" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V52" s="1" t="s">
+      <c r="V52" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="W52" s="1" t="s">
+      <c r="W52" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="X52" s="1">
+      <c r="X52" s="10">
         <v>8</v>
       </c>
     </row>
     <row r="53" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V53" s="1" t="s">
+      <c r="V53" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="W53" s="1" t="s">
+      <c r="W53" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="X53" s="1">
+      <c r="X53" s="10">
         <v>137</v>
       </c>
     </row>
     <row r="54" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V54" s="1" t="s">
+      <c r="V54" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="W54" s="1" t="s">
+      <c r="W54" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="X54" s="1">
+      <c r="X54" s="10">
         <v>1028</v>
       </c>
     </row>
     <row r="55" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V55" s="1" t="s">
+      <c r="V55" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="W55" s="1" t="s">
+      <c r="W55" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="X55" s="1">
+      <c r="X55" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="56" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V56" s="1" t="s">
+      <c r="V56" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="W56" s="1" t="s">
+      <c r="W56" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="X56" s="1">
+      <c r="X56" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="57" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V57" s="1" t="s">
+      <c r="V57" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="W57" s="1" t="s">
+      <c r="W57" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="X57" s="1">
+      <c r="X57" s="10">
         <v>500</v>
       </c>
     </row>
     <row r="58" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V58" s="1" t="s">
+      <c r="V58" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="W58" s="1" t="s">
+      <c r="W58" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="X58" s="1">
+      <c r="X58" s="10">
         <v>238</v>
       </c>
     </row>
     <row r="59" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V59" s="1" t="s">
+      <c r="V59" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="W59" s="1" t="s">
+      <c r="W59" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="X59" s="1">
+      <c r="X59" s="10">
         <v>561</v>
       </c>
     </row>
     <row r="60" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V60" s="1" t="s">
+      <c r="V60" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="W60" s="1" t="s">
+      <c r="W60" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="X60" s="1">
+      <c r="X60" s="10">
         <v>219</v>
       </c>
     </row>
     <row r="61" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V61" s="1" t="s">
+      <c r="V61" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="W61" s="1" t="s">
+      <c r="W61" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="X61" s="1">
+      <c r="X61" s="10">
         <v>2</v>
       </c>
     </row>
     <row r="62" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V62" s="1" t="s">
+      <c r="V62" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="W62" s="1" t="s">
+      <c r="W62" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="X62" s="1">
+      <c r="X62" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="63" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V63" s="1" t="s">
+      <c r="V63" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="W63" s="1" t="s">
+      <c r="W63" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="X63" s="1">
+      <c r="X63" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="64" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V64" s="1" t="s">
+      <c r="V64" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="W64" s="1" t="s">
+      <c r="W64" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="X64" s="1">
+      <c r="X64" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="65" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V65" s="1" t="s">
+      <c r="V65" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="W65" s="1" t="s">
+      <c r="W65" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="X65" s="1">
+      <c r="X65" s="10">
         <v>37</v>
       </c>
     </row>
     <row r="66" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V66" s="1" t="s">
+      <c r="V66" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="W66" s="1" t="s">
+      <c r="W66" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="X66" s="1">
+      <c r="X66" s="10">
         <v>4</v>
       </c>
     </row>
     <row r="67" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V67" s="1" t="s">
+      <c r="V67" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="W67" s="1" t="s">
+      <c r="W67" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="X67" s="1">
+      <c r="X67" s="10">
         <v>155</v>
       </c>
     </row>
     <row r="68" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V68" s="1" t="s">
+      <c r="V68" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="W68" s="1" t="s">
+      <c r="W68" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="X68" s="1">
+      <c r="X68" s="10">
         <v>180</v>
       </c>
     </row>
     <row r="69" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V69" s="1" t="s">
+      <c r="V69" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="W69" s="1" t="s">
+      <c r="W69" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="X69" s="1">
+      <c r="X69" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="70" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V70" s="1" t="s">
+      <c r="V70" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="W70" s="1" t="s">
+      <c r="W70" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="X70" s="1">
+      <c r="X70" s="10">
         <v>1012</v>
       </c>
     </row>
     <row r="71" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V71" s="1" t="s">
+      <c r="V71" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="W71" s="1" t="s">
+      <c r="W71" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="X71" s="1">
+      <c r="X71" s="10">
         <v>680</v>
       </c>
     </row>
     <row r="72" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V72" s="1" t="s">
+      <c r="V72" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="W72" s="1" t="s">
+      <c r="W72" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="X72" s="1">
+      <c r="X72" s="10">
         <v>172</v>
       </c>
     </row>
     <row r="73" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V73" s="1" t="s">
+      <c r="V73" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="W73" s="1" t="s">
+      <c r="W73" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="X73" s="1">
+      <c r="X73" s="10">
         <v>39</v>
       </c>
     </row>
     <row r="74" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V74" s="1" t="s">
+      <c r="V74" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="W74" s="1" t="s">
+      <c r="W74" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="X74" s="1">
+      <c r="X74" s="10">
         <v>291</v>
       </c>
     </row>
     <row r="75" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V75" s="1" t="s">
+      <c r="V75" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="W75" s="1" t="s">
+      <c r="W75" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="X75" s="1">
+      <c r="X75" s="10">
         <v>44</v>
       </c>
     </row>
     <row r="76" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V76" s="1" t="s">
+      <c r="V76" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="W76" s="1" t="s">
+      <c r="W76" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="X76" s="1">
+      <c r="X76" s="10">
         <v>7</v>
       </c>
     </row>
     <row r="77" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V77" s="1" t="s">
+      <c r="V77" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="W77" s="1" t="s">
+      <c r="W77" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="X77" s="1">
+      <c r="X77" s="10">
         <v>155</v>
       </c>
     </row>
     <row r="78" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V78" s="1" t="s">
+      <c r="V78" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="W78" s="1" t="s">
+      <c r="W78" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="X78" s="1">
+      <c r="X78" s="10">
         <v>67</v>
       </c>
     </row>
     <row r="79" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V79" s="1" t="s">
+      <c r="V79" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="W79" s="1">
+      <c r="W79" s="10">
         <v>300</v>
       </c>
-      <c r="X79" s="1">
+      <c r="X79" s="10">
         <v>6</v>
       </c>
     </row>
     <row r="80" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V80" s="1" t="s">
+      <c r="V80" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="W80" s="1" t="s">
+      <c r="W80" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="X80" s="1">
+      <c r="X80" s="10">
         <v>7</v>
       </c>
     </row>
     <row r="81" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V81" s="1" t="s">
+      <c r="V81" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="W81" s="1" t="s">
+      <c r="W81" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="X81" s="1">
+      <c r="X81" s="10">
         <v>6</v>
       </c>
     </row>
     <row r="82" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V82" s="1" t="s">
+      <c r="V82" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="W82" s="1" t="s">
+      <c r="W82" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="X82" s="1">
+      <c r="X82" s="10">
         <v>80</v>
       </c>
     </row>
     <row r="83" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V83" s="1" t="s">
+      <c r="V83" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="W83" s="1" t="s">
+      <c r="W83" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="X83" s="1">
+      <c r="X83" s="10">
         <v>438</v>
       </c>
     </row>
     <row r="84" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V84" s="1" t="s">
+      <c r="V84" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="W84" s="1" t="s">
+      <c r="W84" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="X84" s="1">
+      <c r="X84" s="10">
         <v>250</v>
       </c>
     </row>
     <row r="85" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V85" s="1" t="s">
+      <c r="V85" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="W85" s="1" t="s">
+      <c r="W85" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="X85" s="1">
+      <c r="X85" s="10">
         <v>4</v>
       </c>
     </row>
     <row r="86" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V86" s="1" t="s">
+      <c r="V86" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="W86" s="1" t="s">
+      <c r="W86" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="X86" s="1">
+      <c r="X86" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="87" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V87" s="1" t="s">
+      <c r="V87" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="W87" s="1" t="s">
+      <c r="W87" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="X87" s="1">
+      <c r="X87" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="88" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V88" s="1" t="s">
+      <c r="V88" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="W88" s="1" t="s">
+      <c r="W88" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="X88" s="1">
+      <c r="X88" s="10">
         <v>6</v>
       </c>
     </row>
     <row r="89" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V89" s="1" t="s">
+      <c r="V89" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="W89" s="1" t="s">
+      <c r="W89" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="X89" s="1">
+      <c r="X89" s="10">
         <v>3</v>
       </c>
     </row>
     <row r="90" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V90" s="1" t="s">
+      <c r="V90" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="W90" s="1" t="s">
+      <c r="W90" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="X90" s="1">
+      <c r="X90" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="91" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V91" s="1" t="s">
+      <c r="V91" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="W91" s="1" t="s">
+      <c r="W91" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="X91" s="1">
+      <c r="X91" s="10">
         <v>3</v>
       </c>
     </row>
     <row r="92" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V92" s="1" t="s">
+      <c r="V92" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="W92" s="1" t="s">
+      <c r="W92" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="X92" s="1">
+      <c r="X92" s="10">
         <v>38</v>
       </c>
     </row>
     <row r="93" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V93" s="1" t="s">
+      <c r="V93" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="W93" s="1" t="s">
+      <c r="W93" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="X93" s="1">
+      <c r="X93" s="10">
         <v>29</v>
       </c>
     </row>
     <row r="94" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V94" s="1" t="s">
+      <c r="V94" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="W94" s="1" t="s">
+      <c r="W94" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="X94" s="1">
+      <c r="X94" s="10">
         <v>5</v>
       </c>
     </row>
     <row r="95" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V95" s="1" t="s">
+      <c r="V95" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="W95" s="1" t="s">
+      <c r="W95" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="X95" s="1">
+      <c r="X95" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="96" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V96" s="1" t="s">
+      <c r="V96" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="W96" s="1">
+      <c r="W96" s="10">
         <v>500</v>
       </c>
-      <c r="X96" s="1">
+      <c r="X96" s="10">
         <v>24</v>
       </c>
     </row>
     <row r="97" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V97" s="1" t="s">
+      <c r="V97" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="W97" s="1" t="s">
+      <c r="W97" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="X97" s="1">
+      <c r="X97" s="10">
         <v>145</v>
       </c>
     </row>
     <row r="98" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V98" s="1" t="s">
+      <c r="V98" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="W98" s="1" t="s">
+      <c r="W98" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="X98" s="1">
+      <c r="X98" s="10">
         <v>55</v>
       </c>
     </row>
     <row r="99" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V99" s="1" t="s">
+      <c r="V99" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="W99" s="1" t="s">
+      <c r="W99" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="X99" s="1">
+      <c r="X99" s="10">
         <v>15</v>
       </c>
     </row>
     <row r="100" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V100" s="1" t="s">
+      <c r="V100" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="W100" s="1" t="s">
+      <c r="W100" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="X100" s="1">
+      <c r="X100" s="10">
         <v>120</v>
       </c>
     </row>
     <row r="101" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V101" s="1" t="s">
+      <c r="V101" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="W101" s="1" t="s">
+      <c r="W101" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="X101" s="1">
+      <c r="X101" s="10">
         <v>38</v>
       </c>
     </row>
     <row r="102" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V102" s="1" t="s">
+      <c r="V102" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="W102" s="1" t="s">
+      <c r="W102" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="X102" s="1">
+      <c r="X102" s="10">
         <v>3</v>
       </c>
     </row>
     <row r="103" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V103" s="1" t="s">
+      <c r="V103" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="W103" s="1" t="s">
+      <c r="W103" s="10" t="s">
         <v>153</v>
       </c>
-      <c r="X103" s="1">
+      <c r="X103" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="104" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V104" s="1" t="s">
+      <c r="V104" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="W104" s="1" t="s">
+      <c r="W104" s="10" t="s">
         <v>154</v>
       </c>
-      <c r="X104" s="1">
+      <c r="X104" s="10">
         <v>264</v>
       </c>
     </row>
     <row r="105" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V105" s="1" t="s">
+      <c r="V105" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="W105" s="1" t="s">
+      <c r="W105" s="10" t="s">
         <v>155</v>
       </c>
-      <c r="X105" s="1">
+      <c r="X105" s="10">
         <v>59</v>
       </c>
     </row>
     <row r="106" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V106" s="1" t="s">
+      <c r="V106" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="W106" s="1" t="s">
+      <c r="W106" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="X106" s="1">
+      <c r="X106" s="10">
         <v>220</v>
       </c>
     </row>
     <row r="107" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V107" s="1" t="s">
+      <c r="V107" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="W107" s="1" t="s">
+      <c r="W107" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="X107" s="1">
+      <c r="X107" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="108" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V108" s="1" t="s">
+      <c r="V108" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="W108" s="1" t="s">
+      <c r="W108" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="X108" s="1">
+      <c r="X108" s="10">
         <v>317</v>
       </c>
     </row>
     <row r="109" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V109" s="1" t="s">
+      <c r="V109" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="W109" s="1" t="s">
+      <c r="W109" s="10" t="s">
         <v>159</v>
       </c>
-      <c r="X109" s="1">
+      <c r="X109" s="10">
         <v>86</v>
       </c>
     </row>
     <row r="110" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V110" s="1" t="s">
+      <c r="V110" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="W110" s="1" t="s">
+      <c r="W110" s="10" t="s">
         <v>160</v>
       </c>
-      <c r="X110" s="1">
+      <c r="X110" s="10">
         <v>112</v>
       </c>
     </row>
     <row r="111" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V111" s="1" t="s">
+      <c r="V111" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="W111" s="1" t="s">
+      <c r="W111" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="X111" s="1">
+      <c r="X111" s="10">
         <v>1699</v>
       </c>
     </row>
     <row r="112" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V112" s="1" t="s">
+      <c r="V112" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="W112" s="1" t="s">
+      <c r="W112" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="X112" s="1">
+      <c r="X112" s="10">
         <v>423</v>
       </c>
     </row>
     <row r="113" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V113" s="1" t="s">
+      <c r="V113" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="W113" s="1" t="s">
+      <c r="W113" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="X113" s="1">
+      <c r="X113" s="10">
         <v>493</v>
       </c>
     </row>
     <row r="114" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V114" s="1" t="s">
+      <c r="V114" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="W114" s="1" t="s">
+      <c r="W114" s="10" t="s">
         <v>164</v>
       </c>
-      <c r="X114" s="1">
+      <c r="X114" s="10">
         <v>72</v>
       </c>
     </row>
     <row r="115" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V115" s="1" t="s">
+      <c r="V115" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="W115" s="1" t="s">
+      <c r="W115" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="X115" s="1">
+      <c r="X115" s="10">
         <v>295</v>
       </c>
     </row>
     <row r="116" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V116" s="1" t="s">
+      <c r="V116" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="W116" s="1" t="s">
+      <c r="W116" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="X116" s="1">
+      <c r="X116" s="10">
         <v>131</v>
       </c>
     </row>
     <row r="117" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V117" s="1" t="s">
+      <c r="V117" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="W117" s="1" t="s">
+      <c r="W117" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="X117" s="1">
+      <c r="X117" s="10">
         <v>1385</v>
       </c>
     </row>
     <row r="118" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V118" s="1" t="s">
+      <c r="V118" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="W118" s="1" t="s">
+      <c r="W118" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="X118" s="1">
+      <c r="X118" s="10">
         <v>6</v>
       </c>
     </row>
     <row r="119" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V119" s="1" t="s">
+      <c r="V119" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="W119" s="1" t="s">
+      <c r="W119" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="X119" s="1">
+      <c r="X119" s="10">
         <v>423</v>
       </c>
     </row>
     <row r="120" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V120" s="1" t="s">
+      <c r="V120" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="W120" s="1" t="s">
+      <c r="W120" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="X120" s="1">
+      <c r="X120" s="10">
         <v>30</v>
       </c>
     </row>
     <row r="121" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V121" s="1" t="s">
+      <c r="V121" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="W121" s="1" t="s">
+      <c r="W121" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="X121" s="1">
+      <c r="X121" s="10">
         <v>3</v>
       </c>
     </row>
     <row r="122" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V122" s="1" t="s">
+      <c r="V122" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="W122" s="1" t="s">
+      <c r="W122" s="10" t="s">
         <v>173</v>
       </c>
-      <c r="X122" s="1">
+      <c r="X122" s="10">
         <v>1221</v>
       </c>
     </row>
     <row r="123" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V123" s="1" t="s">
+      <c r="V123" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="W123" s="1" t="s">
+      <c r="W123" s="10" t="s">
         <v>174</v>
       </c>
-      <c r="X123" s="1">
+      <c r="X123" s="10">
         <v>223</v>
       </c>
     </row>
     <row r="124" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V124" s="1" t="s">
+      <c r="V124" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="W124" s="1" t="s">
+      <c r="W124" s="10" t="s">
         <v>175</v>
       </c>
-      <c r="X124" s="1">
+      <c r="X124" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="125" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V125" s="1" t="s">
+      <c r="V125" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="W125" s="1" t="s">
+      <c r="W125" s="10" t="s">
         <v>176</v>
       </c>
-      <c r="X125" s="1">
+      <c r="X125" s="10">
         <v>133</v>
       </c>
     </row>
     <row r="126" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V126" s="1" t="s">
+      <c r="V126" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="W126" s="1" t="s">
+      <c r="W126" s="10" t="s">
         <v>177</v>
       </c>
-      <c r="X126" s="1">
+      <c r="X126" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="127" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V127" s="1" t="s">
+      <c r="V127" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="W127" s="1" t="s">
+      <c r="W127" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="X127" s="1">
+      <c r="X127" s="10">
         <v>968</v>
       </c>
     </row>
     <row r="128" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V128" s="1" t="s">
+      <c r="V128" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="W128" s="1" t="s">
+      <c r="W128" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="X128" s="1">
+      <c r="X128" s="10">
         <v>178</v>
       </c>
     </row>
     <row r="129" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V129" s="1" t="s">
+      <c r="V129" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="W129" s="1" t="s">
+      <c r="W129" s="10" t="s">
         <v>180</v>
       </c>
-      <c r="X129" s="1">
+      <c r="X129" s="10">
         <v>3</v>
       </c>
     </row>
     <row r="130" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V130" s="1" t="s">
+      <c r="V130" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="W130" s="1" t="s">
+      <c r="W130" s="10" t="s">
         <v>181</v>
       </c>
-      <c r="X130" s="1">
+      <c r="X130" s="10">
         <v>95</v>
       </c>
     </row>
     <row r="131" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V131" s="1" t="s">
+      <c r="V131" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="W131" s="1" t="s">
+      <c r="W131" s="10" t="s">
         <v>182</v>
       </c>
-      <c r="X131" s="1">
+      <c r="X131" s="10">
         <v>11</v>
       </c>
     </row>
     <row r="132" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V132" s="1" t="s">
+      <c r="V132" s="10" t="s">
         <v>183</v>
       </c>
-      <c r="W132" s="1" t="s">
+      <c r="W132" s="10" t="s">
         <v>184</v>
       </c>
-      <c r="X132" s="1">
+      <c r="X132" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="133" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V133" s="1" t="s">
+      <c r="V133" s="10" t="s">
         <v>185</v>
       </c>
-      <c r="W133" s="1" t="s">
+      <c r="W133" s="10" t="s">
         <v>186</v>
       </c>
-      <c r="X133" s="1">
+      <c r="X133" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="134" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V134" s="1" t="s">
+      <c r="V134" s="10" t="s">
         <v>187</v>
       </c>
-      <c r="W134" s="1" t="s">
+      <c r="W134" s="10" t="s">
         <v>188</v>
       </c>
-      <c r="X134" s="1">
+      <c r="X134" s="10">
         <v>6</v>
       </c>
     </row>
     <row r="135" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V135" s="1" t="s">
+      <c r="V135" s="10" t="s">
         <v>189</v>
       </c>
-      <c r="W135" s="1">
+      <c r="W135" s="10">
         <v>0</v>
       </c>
-      <c r="X135" s="1">
+      <c r="X135" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="136" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V136" s="1" t="s">
+      <c r="V136" s="10" t="s">
         <v>189</v>
       </c>
-      <c r="W136" s="1" t="s">
+      <c r="W136" s="10" t="s">
         <v>190</v>
       </c>
-      <c r="X136" s="1">
+      <c r="X136" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="137" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V137" s="1" t="s">
+      <c r="V137" s="10" t="s">
         <v>189</v>
       </c>
-      <c r="W137" s="1" t="s">
+      <c r="W137" s="10" t="s">
         <v>191</v>
       </c>
-      <c r="X137" s="1">
+      <c r="X137" s="10">
         <v>133</v>
       </c>
     </row>
     <row r="138" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V138" s="1" t="s">
+      <c r="V138" s="10" t="s">
         <v>189</v>
       </c>
-      <c r="W138" s="1" t="s">
+      <c r="W138" s="10" t="s">
         <v>192</v>
       </c>
-      <c r="X138" s="1">
+      <c r="X138" s="10">
         <v>602</v>
       </c>
     </row>
     <row r="139" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V139" s="1" t="s">
+      <c r="V139" s="10" t="s">
         <v>189</v>
       </c>
-      <c r="W139" s="1" t="s">
+      <c r="W139" s="10" t="s">
         <v>193</v>
       </c>
-      <c r="X139" s="1">
+      <c r="X139" s="10">
         <v>69</v>
       </c>
     </row>
     <row r="140" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V140" s="1" t="s">
+      <c r="V140" s="10" t="s">
         <v>189</v>
       </c>
-      <c r="W140" s="1" t="s">
+      <c r="W140" s="10" t="s">
         <v>194</v>
       </c>
-      <c r="X140" s="1">
+      <c r="X140" s="10">
         <v>240</v>
       </c>
     </row>
     <row r="141" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V141" s="1" t="s">
+      <c r="V141" s="10" t="s">
         <v>189</v>
       </c>
-      <c r="W141" s="1" t="s">
+      <c r="W141" s="10" t="s">
         <v>195</v>
       </c>
-      <c r="X141" s="1">
+      <c r="X141" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="142" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V142" s="1" t="s">
+      <c r="V142" s="10" t="s">
         <v>189</v>
       </c>
-      <c r="W142" s="1" t="s">
+      <c r="W142" s="10" t="s">
         <v>196</v>
       </c>
-      <c r="X142" s="1">
+      <c r="X142" s="10">
         <v>81</v>
       </c>
     </row>
     <row r="143" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V143" s="1" t="s">
+      <c r="V143" s="10" t="s">
         <v>189</v>
       </c>
-      <c r="W143" s="1" t="s">
+      <c r="W143" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="X143" s="1">
+      <c r="X143" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="144" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V144" s="1" t="s">
+      <c r="V144" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="W144" s="1" t="s">
+      <c r="W144" s="10" t="s">
         <v>199</v>
       </c>
-      <c r="X144" s="1">
+      <c r="X144" s="10">
         <v>60</v>
       </c>
     </row>
     <row r="145" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V145" s="1" t="s">
+      <c r="V145" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="W145" s="1" t="s">
+      <c r="W145" s="10" t="s">
         <v>200</v>
       </c>
-      <c r="X145" s="1">
+      <c r="X145" s="10">
         <v>45</v>
       </c>
     </row>
     <row r="146" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V146" s="1" t="s">
+      <c r="V146" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="W146" s="1" t="s">
+      <c r="W146" s="10" t="s">
         <v>201</v>
       </c>
-      <c r="X146" s="1">
+      <c r="X146" s="10">
         <v>38</v>
       </c>
     </row>
     <row r="147" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V147" s="1" t="s">
+      <c r="V147" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="W147" s="1" t="s">
+      <c r="W147" s="10" t="s">
         <v>202</v>
       </c>
-      <c r="X147" s="1">
+      <c r="X147" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="148" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V148" s="1" t="s">
+      <c r="V148" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="W148" s="1" t="s">
+      <c r="W148" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="X148" s="1">
+      <c r="X148" s="10">
         <v>4</v>
       </c>
     </row>
     <row r="149" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V149" s="1" t="s">
+      <c r="V149" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="W149" s="1" t="s">
+      <c r="W149" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="X149" s="1">
+      <c r="X149" s="10">
         <v>768</v>
       </c>
     </row>
     <row r="150" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V150" s="1" t="s">
+      <c r="V150" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="W150" s="1" t="s">
+      <c r="W150" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="X150" s="1">
+      <c r="X150" s="10">
         <v>200</v>
       </c>
     </row>
     <row r="151" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V151" s="1" t="s">
+      <c r="V151" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="W151" s="1" t="s">
+      <c r="W151" s="10" t="s">
         <v>205</v>
       </c>
-      <c r="X151" s="1">
+      <c r="X151" s="10">
         <v>22</v>
       </c>
     </row>
     <row r="152" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V152" s="1" t="s">
+      <c r="V152" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="W152" s="1" t="s">
+      <c r="W152" s="10" t="s">
         <v>206</v>
       </c>
-      <c r="X152" s="1">
+      <c r="X152" s="10">
         <v>45</v>
       </c>
     </row>
     <row r="153" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V153" s="1" t="s">
+      <c r="V153" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="W153" s="1" t="s">
+      <c r="W153" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="X153" s="1">
+      <c r="X153" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="154" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V154" s="1" t="s">
+      <c r="V154" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="W154" s="1" t="s">
+      <c r="W154" s="10" t="s">
         <v>208</v>
       </c>
-      <c r="X154" s="1">
+      <c r="X154" s="10">
         <v>435</v>
       </c>
     </row>
     <row r="155" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V155" s="1" t="s">
+      <c r="V155" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="W155" s="1" t="s">
+      <c r="W155" s="10" t="s">
         <v>209</v>
       </c>
-      <c r="X155" s="1">
+      <c r="X155" s="10">
         <v>19</v>
       </c>
     </row>
     <row r="156" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V156" s="1" t="s">
+      <c r="V156" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="W156" s="1" t="s">
+      <c r="W156" s="10" t="s">
         <v>210</v>
       </c>
-      <c r="X156" s="1">
+      <c r="X156" s="10">
         <v>161</v>
       </c>
     </row>
     <row r="157" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V157" s="1" t="s">
+      <c r="V157" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="W157" s="1" t="s">
+      <c r="W157" s="10" t="s">
         <v>211</v>
       </c>
-      <c r="X157" s="1">
+      <c r="X157" s="10">
         <v>83</v>
       </c>
     </row>
     <row r="158" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V158" s="1" t="s">
+      <c r="V158" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="W158" s="1" t="s">
+      <c r="W158" s="10" t="s">
         <v>212</v>
       </c>
-      <c r="X158" s="1">
+      <c r="X158" s="10">
         <v>45</v>
       </c>
     </row>
     <row r="159" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V159" s="1" t="s">
+      <c r="V159" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="W159" s="1" t="s">
+      <c r="W159" s="10" t="s">
         <v>213</v>
       </c>
-      <c r="X159" s="1">
+      <c r="X159" s="10">
         <v>327</v>
       </c>
     </row>
     <row r="160" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V160" s="1" t="s">
+      <c r="V160" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="W160" s="1" t="s">
+      <c r="W160" s="10" t="s">
         <v>214</v>
       </c>
-      <c r="X160" s="1">
+      <c r="X160" s="10">
         <v>38</v>
       </c>
     </row>
     <row r="161" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V161" s="1" t="s">
+      <c r="V161" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="W161" s="1" t="s">
+      <c r="W161" s="10" t="s">
         <v>215</v>
       </c>
-      <c r="X161" s="1">
+      <c r="X161" s="10">
         <v>41</v>
       </c>
     </row>
     <row r="162" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V162" s="1" t="s">
+      <c r="V162" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="W162" s="1" t="s">
+      <c r="W162" s="10" t="s">
         <v>217</v>
       </c>
-      <c r="X162" s="1">
+      <c r="X162" s="10">
         <v>2</v>
       </c>
     </row>
     <row r="163" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V163" s="1" t="s">
+      <c r="V163" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="W163" s="1" t="s">
+      <c r="W163" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="X163" s="1">
+      <c r="X163" s="10">
         <v>12</v>
       </c>
     </row>
     <row r="164" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V164" s="1" t="s">
+      <c r="V164" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="W164" s="1" t="s">
+      <c r="W164" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="X164" s="1">
+      <c r="X164" s="10">
         <v>65</v>
       </c>
     </row>
     <row r="165" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V165" s="1" t="s">
+      <c r="V165" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="W165" s="1" t="s">
+      <c r="W165" s="10" t="s">
         <v>220</v>
       </c>
-      <c r="X165" s="1">
+      <c r="X165" s="10">
         <v>6</v>
       </c>
     </row>
     <row r="166" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V166" s="1" t="s">
+      <c r="V166" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="W166" s="1" t="s">
+      <c r="W166" s="10" t="s">
         <v>221</v>
       </c>
-      <c r="X166" s="1">
+      <c r="X166" s="10">
         <v>11</v>
       </c>
     </row>
     <row r="167" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V167" s="1" t="s">
+      <c r="V167" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="W167" s="1" t="s">
+      <c r="W167" s="10" t="s">
         <v>222</v>
       </c>
-      <c r="X167" s="1">
+      <c r="X167" s="10">
         <v>4</v>
       </c>
     </row>
     <row r="168" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V168" s="1" t="s">
+      <c r="V168" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="W168" s="1" t="s">
+      <c r="W168" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="X168" s="1">
+      <c r="X168" s="10">
         <v>5</v>
       </c>
     </row>
     <row r="169" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V169" s="1" t="s">
+      <c r="V169" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="W169" s="1" t="s">
+      <c r="W169" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="X169" s="1">
+      <c r="X169" s="10">
         <v>7</v>
       </c>
     </row>
     <row r="170" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V170" s="1" t="s">
+      <c r="V170" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="W170" s="1" t="s">
+      <c r="W170" s="10" t="s">
         <v>225</v>
       </c>
-      <c r="X170" s="1">
+      <c r="X170" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="171" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V171" s="1" t="s">
+      <c r="V171" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="W171" s="1" t="s">
+      <c r="W171" s="10" t="s">
         <v>226</v>
       </c>
-      <c r="X171" s="1">
+      <c r="X171" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="172" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V172" s="1" t="s">
+      <c r="V172" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="W172" s="1" t="s">
+      <c r="W172" s="10" t="s">
         <v>227</v>
       </c>
-      <c r="X172" s="1">
+      <c r="X172" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="173" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V173" s="1" t="s">
+      <c r="V173" s="10" t="s">
         <v>228</v>
       </c>
-      <c r="W173" s="1" t="s">
+      <c r="W173" s="10" t="s">
         <v>229</v>
       </c>
-      <c r="X173" s="1">
+      <c r="X173" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="174" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V174" s="1" t="s">
+      <c r="V174" s="10" t="s">
         <v>228</v>
       </c>
-      <c r="W174" s="1" t="s">
+      <c r="W174" s="10" t="s">
         <v>230</v>
       </c>
-      <c r="X174" s="1">
+      <c r="X174" s="10">
         <v>5</v>
       </c>
     </row>
     <row r="175" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V175" s="1" t="s">
+      <c r="V175" s="10" t="s">
         <v>228</v>
       </c>
-      <c r="W175" s="1" t="s">
+      <c r="W175" s="10" t="s">
         <v>231</v>
       </c>
-      <c r="X175" s="1">
+      <c r="X175" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="176" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V176" s="1" t="s">
+      <c r="V176" s="10" t="s">
         <v>228</v>
       </c>
-      <c r="W176" s="1" t="s">
+      <c r="W176" s="10" t="s">
         <v>232</v>
       </c>
-      <c r="X176" s="1">
+      <c r="X176" s="10">
         <v>2</v>
       </c>
     </row>
     <row r="177" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V177" s="1" t="s">
+      <c r="V177" s="10" t="s">
         <v>233</v>
       </c>
-      <c r="W177" s="1" t="s">
+      <c r="W177" s="10" t="s">
         <v>234</v>
       </c>
-      <c r="X177" s="1">
+      <c r="X177" s="10">
         <v>3</v>
       </c>
     </row>
     <row r="178" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V178" s="1" t="s">
+      <c r="V178" s="10" t="s">
         <v>233</v>
       </c>
-      <c r="W178" s="1" t="s">
+      <c r="W178" s="10" t="s">
         <v>235</v>
       </c>
-      <c r="X178" s="1">
+      <c r="X178" s="10">
         <v>90</v>
       </c>
     </row>
     <row r="179" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V179" s="1" t="s">
+      <c r="V179" s="10" t="s">
         <v>233</v>
       </c>
-      <c r="W179" s="1" t="s">
+      <c r="W179" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="X179" s="1">
+      <c r="X179" s="10">
         <v>4</v>
       </c>
     </row>
     <row r="180" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V180" s="1" t="s">
+      <c r="V180" s="10" t="s">
         <v>233</v>
       </c>
-      <c r="W180" s="1" t="s">
+      <c r="W180" s="10" t="s">
         <v>236</v>
       </c>
-      <c r="X180" s="1">
+      <c r="X180" s="10">
         <v>142</v>
       </c>
     </row>
     <row r="181" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V181" s="1" t="s">
+      <c r="V181" s="10" t="s">
         <v>233</v>
       </c>
-      <c r="W181" s="1" t="s">
+      <c r="W181" s="10" t="s">
         <v>237</v>
       </c>
-      <c r="X181" s="1">
+      <c r="X181" s="10">
         <v>5</v>
       </c>
     </row>
     <row r="182" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V182" s="1" t="s">
+      <c r="V182" s="10" t="s">
         <v>238</v>
       </c>
-      <c r="W182" s="1" t="s">
+      <c r="W182" s="10" t="s">
         <v>239</v>
       </c>
-      <c r="X182" s="1">
+      <c r="X182" s="10">
         <v>6</v>
       </c>
     </row>
     <row r="183" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V183" s="1" t="s">
+      <c r="V183" s="10" t="s">
         <v>240</v>
       </c>
-      <c r="W183" s="1" t="s">
+      <c r="W183" s="10" t="s">
         <v>241</v>
       </c>
-      <c r="X183" s="1">
+      <c r="X183" s="10">
         <v>21</v>
       </c>
     </row>
     <row r="184" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V184" s="1" t="s">
+      <c r="V184" s="10" t="s">
         <v>240</v>
       </c>
-      <c r="W184" s="1" t="s">
+      <c r="W184" s="10" t="s">
         <v>242</v>
       </c>
-      <c r="X184" s="1">
+      <c r="X184" s="10">
         <v>2</v>
       </c>
     </row>
     <row r="185" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V185" s="1" t="s">
+      <c r="V185" s="10" t="s">
         <v>240</v>
       </c>
-      <c r="W185" s="1" t="s">
+      <c r="W185" s="10" t="s">
         <v>243</v>
       </c>
-      <c r="X185" s="1">
+      <c r="X185" s="10">
         <v>2</v>
       </c>
     </row>
     <row r="186" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V186" s="1" t="s">
+      <c r="V186" s="10" t="s">
         <v>240</v>
       </c>
-      <c r="W186" s="1" t="s">
+      <c r="W186" s="10" t="s">
         <v>244</v>
       </c>
-      <c r="X186" s="1">
+      <c r="X186" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="187" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V187" s="1" t="s">
+      <c r="V187" s="10" t="s">
         <v>240</v>
       </c>
-      <c r="W187" s="1" t="s">
+      <c r="W187" s="10" t="s">
         <v>245</v>
       </c>
-      <c r="X187" s="1">
+      <c r="X187" s="10">
         <v>42</v>
       </c>
     </row>
     <row r="188" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V188" s="1" t="s">
+      <c r="V188" s="10" t="s">
         <v>240</v>
       </c>
-      <c r="W188" s="1" t="s">
+      <c r="W188" s="10" t="s">
         <v>246</v>
       </c>
-      <c r="X188" s="1">
+      <c r="X188" s="10">
         <v>8</v>
       </c>
     </row>
     <row r="189" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V189" s="1" t="s">
+      <c r="V189" s="10" t="s">
         <v>240</v>
       </c>
-      <c r="W189" s="1" t="s">
+      <c r="W189" s="10" t="s">
         <v>247</v>
       </c>
-      <c r="X189" s="1">
+      <c r="X189" s="10">
         <v>24</v>
       </c>
     </row>
     <row r="190" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V190" s="1" t="s">
+      <c r="V190" s="10" t="s">
         <v>240</v>
       </c>
-      <c r="W190" s="1" t="s">
+      <c r="W190" s="10" t="s">
         <v>248</v>
       </c>
-      <c r="X190" s="1">
+      <c r="X190" s="10">
         <v>40</v>
       </c>
     </row>
     <row r="191" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V191" s="1" t="s">
+      <c r="V191" s="10" t="s">
         <v>240</v>
       </c>
-      <c r="W191" s="1" t="s">
+      <c r="W191" s="10" t="s">
         <v>249</v>
       </c>
-      <c r="X191" s="1">
+      <c r="X191" s="10">
         <v>48</v>
       </c>
     </row>
     <row r="192" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V192" s="1" t="s">
+      <c r="V192" s="10" t="s">
         <v>240</v>
       </c>
-      <c r="W192" s="1" t="s">
+      <c r="W192" s="10" t="s">
         <v>250</v>
       </c>
-      <c r="X192" s="1">
+      <c r="X192" s="10">
         <v>141</v>
       </c>
     </row>
     <row r="193" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V193" s="1" t="s">
+      <c r="V193" s="10" t="s">
         <v>251</v>
       </c>
-      <c r="W193" s="1" t="s">
+      <c r="W193" s="10" t="s">
         <v>252</v>
       </c>
-      <c r="X193" s="1">
+      <c r="X193" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="194" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V194" s="1" t="s">
+      <c r="V194" s="10" t="s">
         <v>253</v>
       </c>
-      <c r="W194" s="1" t="s">
+      <c r="W194" s="10" t="s">
         <v>254</v>
       </c>
-      <c r="X194" s="1">
+      <c r="X194" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="195" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V195" s="1" t="s">
+      <c r="V195" s="10" t="s">
         <v>253</v>
       </c>
-      <c r="W195" s="1" t="s">
+      <c r="W195" s="10" t="s">
         <v>255</v>
       </c>
-      <c r="X195" s="1">
+      <c r="X195" s="10">
         <v>8</v>
       </c>
     </row>
     <row r="196" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V196" s="1" t="s">
+      <c r="V196" s="10" t="s">
         <v>253</v>
       </c>
-      <c r="W196" s="1" t="s">
+      <c r="W196" s="10" t="s">
         <v>256</v>
       </c>
-      <c r="X196" s="1">
+      <c r="X196" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="197" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V197" s="1" t="s">
+      <c r="V197" s="10" t="s">
         <v>253</v>
       </c>
-      <c r="W197" s="1" t="s">
+      <c r="W197" s="10" t="s">
         <v>257</v>
       </c>
-      <c r="X197" s="1">
+      <c r="X197" s="10">
         <v>9</v>
       </c>
     </row>
     <row r="198" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V198" s="1" t="s">
+      <c r="V198" s="10" t="s">
         <v>253</v>
       </c>
-      <c r="W198" s="1" t="s">
+      <c r="W198" s="10" t="s">
         <v>258</v>
       </c>
-      <c r="X198" s="1">
+      <c r="X198" s="10">
         <v>22</v>
       </c>
     </row>
     <row r="199" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V199" s="1" t="s">
+      <c r="V199" s="10" t="s">
         <v>253</v>
       </c>
-      <c r="W199" s="1" t="s">
+      <c r="W199" s="10" t="s">
         <v>259</v>
       </c>
-      <c r="X199" s="1">
+      <c r="X199" s="10">
         <v>110</v>
       </c>
     </row>
     <row r="200" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V200" s="1" t="s">
+      <c r="V200" s="10" t="s">
         <v>260</v>
       </c>
-      <c r="W200" s="1" t="s">
+      <c r="W200" s="10" t="s">
         <v>261</v>
       </c>
-      <c r="X200" s="1">
+      <c r="X200" s="10">
         <v>2</v>
       </c>
     </row>
     <row r="201" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V201" s="1" t="s">
+      <c r="V201" s="10" t="s">
         <v>260</v>
       </c>
-      <c r="W201" s="1" t="s">
+      <c r="W201" s="10" t="s">
         <v>262</v>
       </c>
-      <c r="X201" s="1">
+      <c r="X201" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="202" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V202" s="1" t="s">
+      <c r="V202" s="10" t="s">
         <v>260</v>
       </c>
-      <c r="W202" s="1" t="s">
+      <c r="W202" s="10" t="s">
         <v>263</v>
       </c>
-      <c r="X202" s="1">
+      <c r="X202" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="203" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V203" s="1" t="s">
+      <c r="V203" s="10" t="s">
         <v>264</v>
       </c>
-      <c r="W203" s="1">
+      <c r="W203" s="10">
         <v>320</v>
       </c>
-      <c r="X203" s="1">
+      <c r="X203" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="204" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V204" s="1" t="s">
+      <c r="V204" s="10" t="s">
         <v>264</v>
       </c>
-      <c r="W204" s="1">
+      <c r="W204" s="10">
         <v>530</v>
       </c>
-      <c r="X204" s="1">
+      <c r="X204" s="10">
         <v>5</v>
       </c>
     </row>
     <row r="205" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V205" s="1" t="s">
+      <c r="V205" s="10" t="s">
         <v>264</v>
       </c>
-      <c r="W205" s="1" t="s">
+      <c r="W205" s="10" t="s">
         <v>265</v>
       </c>
-      <c r="X205" s="1">
+      <c r="X205" s="10">
         <v>13</v>
       </c>
     </row>
     <row r="206" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V206" s="1" t="s">
+      <c r="V206" s="10" t="s">
         <v>266</v>
       </c>
-      <c r="W206" s="1" t="s">
+      <c r="W206" s="10" t="s">
         <v>267</v>
       </c>
-      <c r="X206" s="1">
+      <c r="X206" s="10">
         <v>5</v>
       </c>
     </row>
     <row r="207" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V207" s="1" t="s">
+      <c r="V207" s="10" t="s">
         <v>266</v>
       </c>
-      <c r="W207" s="1" t="s">
+      <c r="W207" s="10" t="s">
         <v>268</v>
       </c>
-      <c r="X207" s="1">
+      <c r="X207" s="10">
         <v>23</v>
       </c>
     </row>
     <row r="208" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V208" s="1" t="s">
+      <c r="V208" s="10" t="s">
         <v>266</v>
       </c>
-      <c r="W208" s="1" t="s">
+      <c r="W208" s="10" t="s">
         <v>269</v>
       </c>
-      <c r="X208" s="1">
+      <c r="X208" s="10">
         <v>15</v>
       </c>
     </row>
     <row r="209" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V209" s="1" t="s">
+      <c r="V209" s="10" t="s">
         <v>266</v>
       </c>
-      <c r="W209" s="1" t="s">
+      <c r="W209" s="10" t="s">
         <v>270</v>
       </c>
-      <c r="X209" s="1">
+      <c r="X209" s="10">
         <v>6</v>
       </c>
     </row>
     <row r="210" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V210" s="1" t="s">
+      <c r="V210" s="10" t="s">
         <v>266</v>
       </c>
-      <c r="W210" s="1" t="s">
+      <c r="W210" s="10" t="s">
         <v>271</v>
       </c>
-      <c r="X210" s="1">
+      <c r="X210" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="211" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V211" s="1" t="s">
+      <c r="V211" s="10" t="s">
         <v>266</v>
       </c>
-      <c r="W211" s="1" t="s">
+      <c r="W211" s="10" t="s">
         <v>272</v>
       </c>
-      <c r="X211" s="1">
+      <c r="X211" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="212" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V212" s="1" t="s">
+      <c r="V212" s="10" t="s">
         <v>266</v>
       </c>
-      <c r="W212" s="1" t="s">
+      <c r="W212" s="10" t="s">
         <v>273</v>
       </c>
-      <c r="X212" s="1">
+      <c r="X212" s="10">
         <v>7</v>
       </c>
     </row>
     <row r="213" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V213" s="1" t="s">
+      <c r="V213" s="10" t="s">
         <v>266</v>
       </c>
-      <c r="W213" s="1" t="s">
+      <c r="W213" s="10" t="s">
         <v>274</v>
       </c>
-      <c r="X213" s="1">
+      <c r="X213" s="10">
         <v>4</v>
       </c>
     </row>
     <row r="214" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V214" s="1" t="s">
+      <c r="V214" s="10" t="s">
         <v>266</v>
       </c>
-      <c r="W214" s="1" t="s">
+      <c r="W214" s="10" t="s">
         <v>275</v>
       </c>
-      <c r="X214" s="1">
+      <c r="X214" s="10">
         <v>20</v>
       </c>
     </row>
     <row r="215" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V215" s="1" t="s">
+      <c r="V215" s="10" t="s">
         <v>266</v>
       </c>
-      <c r="W215" s="1" t="s">
+      <c r="W215" s="10" t="s">
         <v>276</v>
       </c>
-      <c r="X215" s="1">
+      <c r="X215" s="10">
         <v>2</v>
       </c>
     </row>
     <row r="216" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V216" s="1" t="s">
+      <c r="V216" s="10" t="s">
         <v>266</v>
       </c>
-      <c r="W216" s="1" t="s">
+      <c r="W216" s="10" t="s">
         <v>277</v>
       </c>
-      <c r="X216" s="1">
+      <c r="X216" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="217" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V217" s="1" t="s">
+      <c r="V217" s="10" t="s">
         <v>266</v>
       </c>
-      <c r="W217" s="1" t="s">
+      <c r="W217" s="10" t="s">
         <v>278</v>
       </c>
-      <c r="X217" s="1">
+      <c r="X217" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="218" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V218" s="1" t="s">
+      <c r="V218" s="10" t="s">
         <v>266</v>
       </c>
-      <c r="W218" s="1" t="s">
+      <c r="W218" s="10" t="s">
         <v>279</v>
       </c>
-      <c r="X218" s="1">
+      <c r="X218" s="10">
         <v>26</v>
       </c>
     </row>
     <row r="219" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V219" s="1" t="s">
+      <c r="V219" s="10" t="s">
         <v>266</v>
       </c>
-      <c r="W219" s="1" t="s">
+      <c r="W219" s="10" t="s">
         <v>280</v>
       </c>
-      <c r="X219" s="1">
+      <c r="X219" s="10">
         <v>3</v>
       </c>
     </row>
     <row r="220" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V220" s="1" t="s">
+      <c r="V220" s="10" t="s">
         <v>266</v>
       </c>
-      <c r="W220" s="1" t="s">
+      <c r="W220" s="10" t="s">
         <v>281</v>
       </c>
-      <c r="X220" s="1">
+      <c r="X220" s="10">
         <v>2</v>
       </c>
     </row>
     <row r="221" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V221" s="1" t="s">
+      <c r="V221" s="10" t="s">
         <v>266</v>
       </c>
-      <c r="W221" s="1" t="s">
+      <c r="W221" s="10" t="s">
         <v>282</v>
       </c>
-      <c r="X221" s="1">
+      <c r="X221" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="222" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V222" s="1" t="s">
+      <c r="V222" s="10" t="s">
         <v>266</v>
       </c>
-      <c r="W222" s="1" t="s">
+      <c r="W222" s="10" t="s">
         <v>283</v>
       </c>
-      <c r="X222" s="1">
+      <c r="X222" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="223" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V223" s="1" t="s">
+      <c r="V223" s="10" t="s">
         <v>266</v>
       </c>
-      <c r="W223" s="1" t="s">
+      <c r="W223" s="10" t="s">
         <v>284</v>
       </c>
-      <c r="X223" s="1">
+      <c r="X223" s="10">
         <v>2</v>
       </c>
     </row>
     <row r="224" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V224" s="1" t="s">
+      <c r="V224" s="10" t="s">
         <v>266</v>
       </c>
-      <c r="W224" s="1" t="s">
+      <c r="W224" s="10" t="s">
         <v>285</v>
       </c>
-      <c r="X224" s="1">
+      <c r="X224" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="225" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V225" s="1" t="s">
+      <c r="V225" s="10" t="s">
         <v>266</v>
       </c>
-      <c r="W225" s="1" t="s">
+      <c r="W225" s="10" t="s">
         <v>286</v>
       </c>
-      <c r="X225" s="1">
+      <c r="X225" s="10">
         <v>17</v>
       </c>
     </row>
     <row r="226" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V226" s="1" t="s">
+      <c r="V226" s="10" t="s">
         <v>287</v>
       </c>
-      <c r="W226" s="1" t="s">
+      <c r="W226" s="10" t="s">
         <v>288</v>
       </c>
-      <c r="X226" s="1">
+      <c r="X226" s="10">
         <v>13</v>
       </c>
     </row>
     <row r="227" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V227" s="1" t="s">
+      <c r="V227" s="10" t="s">
         <v>289</v>
       </c>
-      <c r="W227" s="1" t="s">
+      <c r="W227" s="10" t="s">
         <v>290</v>
       </c>
-      <c r="X227" s="1">
+      <c r="X227" s="10">
         <v>37</v>
       </c>
     </row>
     <row r="228" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V228" s="1" t="s">
+      <c r="V228" s="10" t="s">
         <v>289</v>
       </c>
-      <c r="W228" s="1" t="s">
+      <c r="W228" s="10" t="s">
         <v>291</v>
       </c>
-      <c r="X228" s="1">
+      <c r="X228" s="10">
         <v>2</v>
       </c>
     </row>
     <row r="229" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V229" s="1" t="s">
+      <c r="V229" s="10" t="s">
         <v>289</v>
       </c>
-      <c r="W229" s="1" t="s">
+      <c r="W229" s="10" t="s">
         <v>292</v>
       </c>
-      <c r="X229" s="1">
+      <c r="X229" s="10">
         <v>2</v>
       </c>
     </row>
     <row r="230" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V230" s="1" t="s">
+      <c r="V230" s="10" t="s">
         <v>289</v>
       </c>
-      <c r="W230" s="1" t="s">
+      <c r="W230" s="10" t="s">
         <v>293</v>
       </c>
-      <c r="X230" s="1">
+      <c r="X230" s="10">
         <v>53</v>
       </c>
     </row>
     <row r="231" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V231" s="1" t="s">
+      <c r="V231" s="10" t="s">
         <v>289</v>
       </c>
-      <c r="W231" s="1" t="s">
+      <c r="W231" s="10" t="s">
         <v>294</v>
       </c>
-      <c r="X231" s="1">
+      <c r="X231" s="10">
         <v>24</v>
       </c>
     </row>
     <row r="232" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V232" s="1" t="s">
+      <c r="V232" s="10" t="s">
         <v>289</v>
       </c>
-      <c r="W232" s="1" t="s">
+      <c r="W232" s="10" t="s">
         <v>295</v>
       </c>
-      <c r="X232" s="1">
+      <c r="X232" s="10">
         <v>26</v>
       </c>
     </row>
     <row r="233" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V233" s="1" t="s">
+      <c r="V233" s="10" t="s">
         <v>289</v>
       </c>
-      <c r="W233" s="1" t="s">
+      <c r="W233" s="10" t="s">
         <v>296</v>
       </c>
-      <c r="X233" s="1">
+      <c r="X233" s="10">
         <v>32</v>
       </c>
     </row>
     <row r="234" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V234" s="1" t="s">
+      <c r="V234" s="10" t="s">
         <v>297</v>
       </c>
-      <c r="W234" s="1" t="s">
+      <c r="W234" s="10" t="s">
         <v>298</v>
       </c>
-      <c r="X234" s="1">
+      <c r="X234" s="10">
         <v>42</v>
       </c>
     </row>
     <row r="235" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V235" s="1" t="s">
+      <c r="V235" s="10" t="s">
         <v>297</v>
       </c>
-      <c r="W235" s="1" t="s">
+      <c r="W235" s="10" t="s">
         <v>299</v>
       </c>
-      <c r="X235" s="1">
+      <c r="X235" s="10">
         <v>44</v>
       </c>
     </row>
     <row r="236" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V236" s="1" t="s">
+      <c r="V236" s="10" t="s">
         <v>297</v>
       </c>
-      <c r="W236" s="1" t="s">
+      <c r="W236" s="10" t="s">
         <v>300</v>
       </c>
-      <c r="X236" s="1">
+      <c r="X236" s="10">
         <v>77</v>
       </c>
     </row>
     <row r="237" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V237" s="1" t="s">
+      <c r="V237" s="10" t="s">
         <v>297</v>
       </c>
-      <c r="W237" s="1" t="s">
+      <c r="W237" s="10" t="s">
         <v>301</v>
       </c>
-      <c r="X237" s="1">
+      <c r="X237" s="10">
         <v>101</v>
       </c>
     </row>
     <row r="238" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V238" s="1" t="s">
+      <c r="V238" s="10" t="s">
         <v>297</v>
       </c>
-      <c r="W238" s="1" t="s">
+      <c r="W238" s="10" t="s">
         <v>302</v>
       </c>
-      <c r="X238" s="1">
+      <c r="X238" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="239" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V239" s="1" t="s">
+      <c r="V239" s="10" t="s">
         <v>297</v>
       </c>
-      <c r="W239" s="1" t="s">
+      <c r="W239" s="10" t="s">
         <v>303</v>
       </c>
-      <c r="X239" s="1">
+      <c r="X239" s="10">
         <v>98</v>
       </c>
     </row>
     <row r="240" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V240" s="1" t="s">
+      <c r="V240" s="10" t="s">
         <v>297</v>
       </c>
-      <c r="W240" s="1" t="s">
+      <c r="W240" s="10" t="s">
         <v>304</v>
       </c>
-      <c r="X240" s="1">
+      <c r="X240" s="10">
         <v>69</v>
       </c>
     </row>
     <row r="241" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V241" s="1" t="s">
+      <c r="V241" s="10" t="s">
         <v>297</v>
       </c>
-      <c r="W241" s="1" t="s">
+      <c r="W241" s="10" t="s">
         <v>305</v>
       </c>
-      <c r="X241" s="1">
+      <c r="X241" s="10">
         <v>210</v>
       </c>
     </row>
     <row r="242" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V242" s="1" t="s">
+      <c r="V242" s="10" t="s">
         <v>297</v>
       </c>
-      <c r="W242" s="1" t="s">
+      <c r="W242" s="10" t="s">
         <v>306</v>
       </c>
-      <c r="X242" s="1">
+      <c r="X242" s="10">
         <v>2</v>
       </c>
     </row>
     <row r="243" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V243" s="1" t="s">
+      <c r="V243" s="10" t="s">
         <v>307</v>
       </c>
-      <c r="W243" s="1">
+      <c r="W243" s="10">
         <v>2008</v>
       </c>
-      <c r="X243" s="1">
+      <c r="X243" s="10">
         <v>17</v>
       </c>
     </row>
     <row r="244" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V244" s="1" t="s">
+      <c r="V244" s="10" t="s">
         <v>307</v>
       </c>
-      <c r="W244" s="1">
+      <c r="W244" s="10">
         <v>206</v>
       </c>
-      <c r="X244" s="1">
+      <c r="X244" s="10">
         <v>91</v>
       </c>
     </row>
     <row r="245" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V245" s="1" t="s">
+      <c r="V245" s="10" t="s">
         <v>307</v>
       </c>
-      <c r="W245" s="1">
+      <c r="W245" s="10">
         <v>207</v>
       </c>
-      <c r="X245" s="1">
+      <c r="X245" s="10">
         <v>467</v>
       </c>
     </row>
     <row r="246" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V246" s="1" t="s">
+      <c r="V246" s="10" t="s">
         <v>307</v>
       </c>
-      <c r="W246" s="1">
+      <c r="W246" s="10">
         <v>208</v>
       </c>
-      <c r="X246" s="1">
+      <c r="X246" s="10">
         <v>65</v>
       </c>
     </row>
     <row r="247" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V247" s="1" t="s">
+      <c r="V247" s="10" t="s">
         <v>307</v>
       </c>
-      <c r="W247" s="1">
+      <c r="W247" s="10">
         <v>3008</v>
       </c>
-      <c r="X247" s="1">
+      <c r="X247" s="10">
         <v>12</v>
       </c>
     </row>
     <row r="248" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V248" s="1" t="s">
+      <c r="V248" s="10" t="s">
         <v>307</v>
       </c>
-      <c r="W248" s="1">
+      <c r="W248" s="10">
         <v>307</v>
       </c>
-      <c r="X248" s="1">
+      <c r="X248" s="10">
         <v>128</v>
       </c>
     </row>
     <row r="249" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V249" s="1" t="s">
+      <c r="V249" s="10" t="s">
         <v>307</v>
       </c>
-      <c r="W249" s="1">
+      <c r="W249" s="10">
         <v>308</v>
       </c>
-      <c r="X249" s="1">
+      <c r="X249" s="10">
         <v>44</v>
       </c>
     </row>
     <row r="250" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V250" s="1" t="s">
+      <c r="V250" s="10" t="s">
         <v>307</v>
       </c>
-      <c r="W250" s="1">
+      <c r="W250" s="10">
         <v>407</v>
       </c>
-      <c r="X250" s="1">
+      <c r="X250" s="10">
         <v>2</v>
       </c>
     </row>
     <row r="251" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V251" s="1" t="s">
+      <c r="V251" s="10" t="s">
         <v>307</v>
       </c>
-      <c r="W251" s="1">
+      <c r="W251" s="10">
         <v>408</v>
       </c>
-      <c r="X251" s="1">
+      <c r="X251" s="10">
         <v>34</v>
       </c>
     </row>
     <row r="252" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V252" s="1" t="s">
+      <c r="V252" s="10" t="s">
         <v>307</v>
       </c>
-      <c r="W252" s="1">
+      <c r="W252" s="10">
         <v>5008</v>
       </c>
-      <c r="X252" s="1">
+      <c r="X252" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="253" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V253" s="1" t="s">
+      <c r="V253" s="10" t="s">
         <v>307</v>
       </c>
-      <c r="W253" s="1">
+      <c r="W253" s="10">
         <v>508</v>
       </c>
-      <c r="X253" s="1">
+      <c r="X253" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="254" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V254" s="1" t="s">
+      <c r="V254" s="10" t="s">
         <v>307</v>
       </c>
-      <c r="W254" s="1" t="s">
+      <c r="W254" s="10" t="s">
         <v>308</v>
       </c>
-      <c r="X254" s="1">
+      <c r="X254" s="10">
         <v>2</v>
       </c>
     </row>
     <row r="255" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V255" s="1" t="s">
+      <c r="V255" s="10" t="s">
         <v>307</v>
       </c>
-      <c r="W255" s="1" t="s">
+      <c r="W255" s="10" t="s">
         <v>309</v>
       </c>
-      <c r="X255" s="1">
+      <c r="X255" s="10">
         <v>6</v>
       </c>
     </row>
     <row r="256" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V256" s="1" t="s">
+      <c r="V256" s="10" t="s">
         <v>307</v>
       </c>
-      <c r="W256" s="1" t="s">
+      <c r="W256" s="10" t="s">
         <v>310</v>
       </c>
-      <c r="X256" s="1">
+      <c r="X256" s="10">
         <v>10</v>
       </c>
     </row>
     <row r="257" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V257" s="1" t="s">
+      <c r="V257" s="10" t="s">
         <v>307</v>
       </c>
-      <c r="W257" s="1" t="s">
+      <c r="W257" s="10" t="s">
         <v>311</v>
       </c>
-      <c r="X257" s="1">
+      <c r="X257" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="258" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V258" s="1" t="s">
+      <c r="V258" s="10" t="s">
         <v>312</v>
       </c>
-      <c r="W258" s="1" t="s">
+      <c r="W258" s="10" t="s">
         <v>313</v>
       </c>
-      <c r="X258" s="1">
+      <c r="X258" s="10">
         <v>5</v>
       </c>
     </row>
     <row r="259" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V259" s="1" t="s">
+      <c r="V259" s="10" t="s">
         <v>312</v>
       </c>
-      <c r="W259" s="1" t="s">
+      <c r="W259" s="10" t="s">
         <v>314</v>
       </c>
-      <c r="X259" s="1">
+      <c r="X259" s="10">
         <v>12</v>
       </c>
     </row>
     <row r="260" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V260" s="1" t="s">
+      <c r="V260" s="10" t="s">
         <v>312</v>
       </c>
-      <c r="W260" s="1" t="s">
+      <c r="W260" s="10" t="s">
         <v>315</v>
       </c>
-      <c r="X260" s="1">
+      <c r="X260" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="261" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V261" s="1" t="s">
+      <c r="V261" s="10" t="s">
         <v>312</v>
       </c>
-      <c r="W261" s="1" t="s">
+      <c r="W261" s="10" t="s">
         <v>316</v>
       </c>
-      <c r="X261" s="1">
+      <c r="X261" s="10">
         <v>3</v>
       </c>
     </row>
     <row r="262" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V262" s="1" t="s">
+      <c r="V262" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="W262" s="1">
+      <c r="W262" s="10">
         <v>2500</v>
       </c>
-      <c r="X262" s="1">
+      <c r="X262" s="10">
         <v>4</v>
       </c>
     </row>
     <row r="263" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V263" s="1" t="s">
+      <c r="V263" s="10" t="s">
         <v>317</v>
       </c>
-      <c r="W263" s="1" t="s">
+      <c r="W263" s="10" t="s">
         <v>318</v>
       </c>
-      <c r="X263" s="1">
+      <c r="X263" s="10">
         <v>17</v>
       </c>
     </row>
     <row r="264" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V264" s="1" t="s">
+      <c r="V264" s="10" t="s">
         <v>317</v>
       </c>
-      <c r="W264" s="1" t="s">
+      <c r="W264" s="10" t="s">
         <v>319</v>
       </c>
-      <c r="X264" s="1">
+      <c r="X264" s="10">
         <v>192</v>
       </c>
     </row>
     <row r="265" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V265" s="1" t="s">
+      <c r="V265" s="10" t="s">
         <v>317</v>
       </c>
-      <c r="W265" s="1" t="s">
+      <c r="W265" s="10" t="s">
         <v>320</v>
       </c>
-      <c r="X265" s="1">
+      <c r="X265" s="10">
         <v>152</v>
       </c>
     </row>
     <row r="266" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V266" s="1" t="s">
+      <c r="V266" s="10" t="s">
         <v>317</v>
       </c>
-      <c r="W266" s="1" t="s">
+      <c r="W266" s="10" t="s">
         <v>321</v>
       </c>
-      <c r="X266" s="1">
+      <c r="X266" s="10">
         <v>52</v>
       </c>
     </row>
     <row r="267" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V267" s="1" t="s">
+      <c r="V267" s="10" t="s">
         <v>317</v>
       </c>
-      <c r="W267" s="1" t="s">
+      <c r="W267" s="10" t="s">
         <v>322</v>
       </c>
-      <c r="X267" s="1">
+      <c r="X267" s="10">
         <v>28</v>
       </c>
     </row>
     <row r="268" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V268" s="1" t="s">
+      <c r="V268" s="10" t="s">
         <v>317</v>
       </c>
-      <c r="W268" s="1" t="s">
+      <c r="W268" s="10" t="s">
         <v>323</v>
       </c>
-      <c r="X268" s="1">
+      <c r="X268" s="10">
         <v>111</v>
       </c>
     </row>
     <row r="269" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V269" s="1" t="s">
+      <c r="V269" s="10" t="s">
         <v>317</v>
       </c>
-      <c r="W269" s="1" t="s">
+      <c r="W269" s="10" t="s">
         <v>324</v>
       </c>
-      <c r="X269" s="1">
+      <c r="X269" s="10">
         <v>639</v>
       </c>
     </row>
     <row r="270" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V270" s="1" t="s">
+      <c r="V270" s="10" t="s">
         <v>317</v>
       </c>
-      <c r="W270" s="1" t="s">
+      <c r="W270" s="10" t="s">
         <v>325</v>
       </c>
-      <c r="X270" s="1">
+      <c r="X270" s="10">
         <v>33</v>
       </c>
     </row>
     <row r="271" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V271" s="1" t="s">
+      <c r="V271" s="10" t="s">
         <v>317</v>
       </c>
-      <c r="W271" s="1" t="s">
+      <c r="W271" s="10" t="s">
         <v>326</v>
       </c>
-      <c r="X271" s="1">
+      <c r="X271" s="10">
         <v>92</v>
       </c>
     </row>
     <row r="272" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V272" s="1" t="s">
+      <c r="V272" s="10" t="s">
         <v>317</v>
       </c>
-      <c r="W272" s="1" t="s">
+      <c r="W272" s="10" t="s">
         <v>327</v>
       </c>
-      <c r="X272" s="1">
+      <c r="X272" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="273" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V273" s="1" t="s">
+      <c r="V273" s="10" t="s">
         <v>317</v>
       </c>
-      <c r="W273" s="1" t="s">
+      <c r="W273" s="10" t="s">
         <v>328</v>
       </c>
-      <c r="X273" s="1">
+      <c r="X273" s="10">
         <v>1039</v>
       </c>
     </row>
     <row r="274" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V274" s="1" t="s">
+      <c r="V274" s="10" t="s">
         <v>317</v>
       </c>
-      <c r="W274" s="1" t="s">
+      <c r="W274" s="10" t="s">
         <v>329</v>
       </c>
-      <c r="X274" s="1">
+      <c r="X274" s="10">
         <v>11</v>
       </c>
     </row>
     <row r="275" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V275" s="1" t="s">
+      <c r="V275" s="10" t="s">
         <v>317</v>
       </c>
-      <c r="W275" s="1" t="s">
+      <c r="W275" s="10" t="s">
         <v>330</v>
       </c>
-      <c r="X275" s="1">
+      <c r="X275" s="10">
         <v>2</v>
       </c>
     </row>
     <row r="276" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V276" s="1" t="s">
+      <c r="V276" s="10" t="s">
         <v>317</v>
       </c>
-      <c r="W276" s="1" t="s">
+      <c r="W276" s="10" t="s">
         <v>331</v>
       </c>
-      <c r="X276" s="1">
+      <c r="X276" s="10">
         <v>39</v>
       </c>
     </row>
     <row r="277" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V277" s="1" t="s">
+      <c r="V277" s="10" t="s">
         <v>332</v>
       </c>
-      <c r="W277" s="1" t="s">
+      <c r="W277" s="10" t="s">
         <v>333</v>
       </c>
-      <c r="X277" s="1">
+      <c r="X277" s="10">
         <v>2</v>
       </c>
     </row>
     <row r="278" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V278" s="1" t="s">
+      <c r="V278" s="10" t="s">
         <v>334</v>
       </c>
-      <c r="W278" s="1" t="s">
+      <c r="W278" s="10" t="s">
         <v>335</v>
       </c>
-      <c r="X278" s="1">
+      <c r="X278" s="10">
         <v>3</v>
       </c>
     </row>
     <row r="279" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V279" s="1" t="s">
+      <c r="V279" s="10" t="s">
         <v>334</v>
       </c>
-      <c r="W279" s="1" t="s">
+      <c r="W279" s="10" t="s">
         <v>336</v>
       </c>
-      <c r="X279" s="1">
+      <c r="X279" s="10">
         <v>4</v>
       </c>
     </row>
     <row r="280" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V280" s="1" t="s">
+      <c r="V280" s="10" t="s">
         <v>337</v>
       </c>
-      <c r="W280" s="1" t="s">
+      <c r="W280" s="10" t="s">
         <v>338</v>
       </c>
-      <c r="X280" s="1">
+      <c r="X280" s="10">
         <v>5</v>
       </c>
     </row>
     <row r="281" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V281" s="1" t="s">
+      <c r="V281" s="10" t="s">
         <v>339</v>
       </c>
-      <c r="W281" s="1" t="s">
+      <c r="W281" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="X281" s="1">
+      <c r="X281" s="10">
         <v>8</v>
       </c>
     </row>
     <row r="282" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V282" s="1" t="s">
+      <c r="V282" s="10" t="s">
         <v>339</v>
       </c>
-      <c r="W282" s="1" t="s">
+      <c r="W282" s="10" t="s">
         <v>340</v>
       </c>
-      <c r="X282" s="1">
+      <c r="X282" s="10">
         <v>4</v>
       </c>
     </row>
     <row r="283" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V283" s="1" t="s">
+      <c r="V283" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="W283" s="1" t="s">
+      <c r="W283" s="10" t="s">
         <v>342</v>
       </c>
-      <c r="X283" s="1">
+      <c r="X283" s="10">
         <v>3</v>
       </c>
     </row>
     <row r="284" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V284" s="1" t="s">
+      <c r="V284" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="W284" s="1" t="s">
+      <c r="W284" s="10" t="s">
         <v>343</v>
       </c>
-      <c r="X284" s="1">
+      <c r="X284" s="10">
         <v>303</v>
       </c>
     </row>
     <row r="285" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V285" s="1" t="s">
+      <c r="V285" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="W285" s="1" t="s">
+      <c r="W285" s="10" t="s">
         <v>344</v>
       </c>
-      <c r="X285" s="1">
+      <c r="X285" s="10">
         <v>146</v>
       </c>
     </row>
     <row r="286" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V286" s="1" t="s">
+      <c r="V286" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="W286" s="1" t="s">
+      <c r="W286" s="10" t="s">
         <v>345</v>
       </c>
-      <c r="X286" s="1">
+      <c r="X286" s="10">
         <v>113</v>
       </c>
     </row>
     <row r="287" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V287" s="1" t="s">
+      <c r="V287" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="W287" s="1" t="s">
+      <c r="W287" s="10" t="s">
         <v>346</v>
       </c>
-      <c r="X287" s="1">
+      <c r="X287" s="10">
         <v>2</v>
       </c>
     </row>
     <row r="288" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V288" s="1" t="s">
+      <c r="V288" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="W288" s="1" t="s">
+      <c r="W288" s="10" t="s">
         <v>347</v>
       </c>
-      <c r="X288" s="1">
+      <c r="X288" s="10">
         <v>8</v>
       </c>
     </row>
     <row r="289" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V289" s="1" t="s">
+      <c r="V289" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="W289" s="1" t="s">
+      <c r="W289" s="10" t="s">
         <v>348</v>
       </c>
-      <c r="X289" s="1">
+      <c r="X289" s="10">
         <v>5</v>
       </c>
     </row>
     <row r="290" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V290" s="1" t="s">
+      <c r="V290" s="10" t="s">
         <v>349</v>
       </c>
-      <c r="W290" s="1" t="s">
+      <c r="W290" s="10" t="s">
         <v>350</v>
       </c>
-      <c r="X290" s="1">
+      <c r="X290" s="10">
         <v>4</v>
       </c>
     </row>
     <row r="291" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V291" s="1" t="s">
+      <c r="V291" s="10" t="s">
         <v>351</v>
       </c>
-      <c r="W291" s="1">
+      <c r="W291" s="10">
         <v>0</v>
       </c>
-      <c r="X291" s="1">
+      <c r="X291" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="292" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V292" s="1" t="s">
+      <c r="V292" s="10" t="s">
         <v>351</v>
       </c>
-      <c r="W292" s="1" t="s">
+      <c r="W292" s="10" t="s">
         <v>352</v>
       </c>
-      <c r="X292" s="1">
+      <c r="X292" s="10">
         <v>84</v>
       </c>
     </row>
     <row r="293" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V293" s="1" t="s">
+      <c r="V293" s="10" t="s">
         <v>351</v>
       </c>
-      <c r="W293" s="1" t="s">
+      <c r="W293" s="10" t="s">
         <v>353</v>
       </c>
-      <c r="X293" s="1">
+      <c r="X293" s="10">
         <v>14</v>
       </c>
     </row>
     <row r="294" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V294" s="1" t="s">
+      <c r="V294" s="10" t="s">
         <v>351</v>
       </c>
-      <c r="W294" s="1" t="s">
+      <c r="W294" s="10" t="s">
         <v>354</v>
       </c>
-      <c r="X294" s="1">
+      <c r="X294" s="10">
         <v>76</v>
       </c>
     </row>
     <row r="295" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V295" s="1" t="s">
+      <c r="V295" s="10" t="s">
         <v>351</v>
       </c>
-      <c r="W295" s="1" t="s">
+      <c r="W295" s="10" t="s">
         <v>355</v>
       </c>
-      <c r="X295" s="1">
+      <c r="X295" s="10">
         <v>983</v>
       </c>
     </row>
     <row r="296" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V296" s="1" t="s">
+      <c r="V296" s="10" t="s">
         <v>351</v>
       </c>
-      <c r="W296" s="1" t="s">
+      <c r="W296" s="10" t="s">
         <v>356</v>
       </c>
-      <c r="X296" s="1">
+      <c r="X296" s="10">
         <v>7</v>
       </c>
     </row>
     <row r="297" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V297" s="1" t="s">
+      <c r="V297" s="10" t="s">
         <v>351</v>
       </c>
-      <c r="W297" s="1" t="s">
+      <c r="W297" s="10" t="s">
         <v>357</v>
       </c>
-      <c r="X297" s="1">
+      <c r="X297" s="10">
         <v>1547</v>
       </c>
     </row>
     <row r="298" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V298" s="1" t="s">
+      <c r="V298" s="10" t="s">
         <v>351</v>
       </c>
-      <c r="W298" s="1" t="s">
+      <c r="W298" s="10" t="s">
         <v>358</v>
       </c>
-      <c r="X298" s="1">
+      <c r="X298" s="10">
         <v>186</v>
       </c>
     </row>
     <row r="299" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V299" s="1" t="s">
+      <c r="V299" s="10" t="s">
         <v>351</v>
       </c>
-      <c r="W299" s="1" t="s">
+      <c r="W299" s="10" t="s">
         <v>359</v>
       </c>
-      <c r="X299" s="1">
+      <c r="X299" s="10">
         <v>189</v>
       </c>
     </row>
     <row r="300" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V300" s="1" t="s">
+      <c r="V300" s="10" t="s">
         <v>351</v>
       </c>
-      <c r="W300" s="1" t="s">
+      <c r="W300" s="10" t="s">
         <v>360</v>
       </c>
-      <c r="X300" s="1">
+      <c r="X300" s="10">
         <v>42</v>
       </c>
     </row>
     <row r="301" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V301" s="1" t="s">
+      <c r="V301" s="10" t="s">
         <v>351</v>
       </c>
-      <c r="W301" s="1" t="s">
+      <c r="W301" s="10" t="s">
         <v>361</v>
       </c>
-      <c r="X301" s="1">
+      <c r="X301" s="10">
         <v>18</v>
       </c>
     </row>
     <row r="302" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V302" s="1" t="s">
+      <c r="V302" s="10" t="s">
         <v>351</v>
       </c>
-      <c r="W302" s="1" t="s">
+      <c r="W302" s="10" t="s">
         <v>362</v>
       </c>
-      <c r="X302" s="1">
+      <c r="X302" s="10">
         <v>16</v>
       </c>
     </row>
     <row r="303" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V303" s="1" t="s">
+      <c r="V303" s="10" t="s">
         <v>351</v>
       </c>
-      <c r="W303" s="1" t="s">
+      <c r="W303" s="10" t="s">
         <v>363</v>
       </c>
-      <c r="X303" s="1">
+      <c r="X303" s="10">
         <v>35</v>
       </c>
     </row>
     <row r="304" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V304" s="1" t="s">
+      <c r="V304" s="10" t="s">
         <v>351</v>
       </c>
-      <c r="W304" s="1" t="s">
+      <c r="W304" s="10" t="s">
         <v>364</v>
       </c>
-      <c r="X304" s="1">
+      <c r="X304" s="10">
         <v>15</v>
       </c>
     </row>
     <row r="305" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V305" s="1" t="s">
+      <c r="V305" s="10" t="s">
         <v>351</v>
       </c>
-      <c r="W305" s="1" t="s">
+      <c r="W305" s="10" t="s">
         <v>365</v>
       </c>
-      <c r="X305" s="1">
+      <c r="X305" s="10">
         <v>227</v>
       </c>
     </row>
     <row r="306" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V306" s="1" t="s">
+      <c r="V306" s="10" t="s">
         <v>351</v>
       </c>
-      <c r="W306" s="1" t="s">
+      <c r="W306" s="10" t="s">
         <v>366</v>
       </c>
-      <c r="X306" s="1">
+      <c r="X306" s="10">
         <v>280</v>
       </c>
     </row>
     <row r="307" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V307" s="1" t="s">
+      <c r="V307" s="10" t="s">
         <v>351</v>
       </c>
-      <c r="W307" s="1" t="s">
+      <c r="W307" s="10" t="s">
         <v>367</v>
       </c>
-      <c r="X307" s="1">
+      <c r="X307" s="10">
         <v>7</v>
       </c>
     </row>
     <row r="308" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V308" s="1" t="s">
+      <c r="V308" s="10" t="s">
         <v>351</v>
       </c>
-      <c r="W308" s="1" t="s">
+      <c r="W308" s="10" t="s">
         <v>368</v>
       </c>
-      <c r="X308" s="1">
+      <c r="X308" s="10">
         <v>153</v>
       </c>
     </row>
     <row r="309" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V309" s="1" t="s">
+      <c r="V309" s="10" t="s">
         <v>351</v>
       </c>
-      <c r="W309" s="1" t="s">
+      <c r="W309" s="10" t="s">
         <v>369</v>
       </c>
-      <c r="X309" s="1">
+      <c r="X309" s="10">
         <v>18</v>
       </c>
     </row>
     <row r="310" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V310" s="1" t="s">
+      <c r="V310" s="10" t="s">
         <v>351</v>
       </c>
-      <c r="W310" s="1" t="s">
+      <c r="W310" s="10" t="s">
         <v>370</v>
       </c>
-      <c r="X310" s="1">
+      <c r="X310" s="10">
         <v>62</v>
       </c>
     </row>
     <row r="311" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V311" s="1" t="s">
+      <c r="V311" s="10" t="s">
         <v>351</v>
       </c>
-      <c r="W311" s="1" t="s">
+      <c r="W311" s="10" t="s">
         <v>371</v>
       </c>
-      <c r="X311" s="1">
+      <c r="X311" s="10">
         <v>2</v>
       </c>
     </row>
     <row r="312" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V312" s="1" t="s">
+      <c r="V312" s="10" t="s">
         <v>351</v>
       </c>
-      <c r="W312" s="1" t="s">
+      <c r="W312" s="10" t="s">
         <v>372</v>
       </c>
-      <c r="X312" s="1">
+      <c r="X312" s="10">
         <v>150</v>
       </c>
     </row>
     <row r="313" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V313" s="1" t="s">
+      <c r="V313" s="10" t="s">
         <v>351</v>
       </c>
-      <c r="W313" s="1" t="s">
+      <c r="W313" s="10" t="s">
         <v>373</v>
       </c>
-      <c r="X313" s="1">
+      <c r="X313" s="10">
         <v>50</v>
       </c>
     </row>
     <row r="314" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V314" s="1" t="s">
+      <c r="V314" s="10" t="s">
         <v>351</v>
       </c>
-      <c r="W314" s="1" t="s">
+      <c r="W314" s="10" t="s">
         <v>374</v>
       </c>
-      <c r="X314" s="1">
+      <c r="X314" s="10">
         <v>637</v>
       </c>
     </row>
     <row r="315" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V315" s="1" t="s">
+      <c r="V315" s="10" t="s">
         <v>351</v>
       </c>
-      <c r="W315" s="1" t="s">
+      <c r="W315" s="10" t="s">
         <v>375</v>
       </c>
-      <c r="X315" s="1">
+      <c r="X315" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="316" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V316" s="1" t="s">
+      <c r="V316" s="10" t="s">
         <v>351</v>
       </c>
-      <c r="W316" s="1" t="s">
+      <c r="W316" s="10" t="s">
         <v>376</v>
       </c>
-      <c r="X316" s="1">
+      <c r="X316" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="317" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V317" s="1" t="s">
+      <c r="V317" s="10" t="s">
         <v>377</v>
       </c>
-      <c r="W317" s="1" t="s">
+      <c r="W317" s="10" t="s">
         <v>378</v>
       </c>
-      <c r="X317" s="1">
+      <c r="X317" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="318" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V318" s="1" t="s">
+      <c r="V318" s="10" t="s">
         <v>377</v>
       </c>
-      <c r="W318" s="1" t="s">
+      <c r="W318" s="10" t="s">
         <v>379</v>
       </c>
-      <c r="X318" s="1">
+      <c r="X318" s="10">
         <v>7</v>
       </c>
     </row>
     <row r="319" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V319" s="1" t="s">
+      <c r="V319" s="10" t="s">
         <v>377</v>
       </c>
-      <c r="W319" s="1" t="s">
+      <c r="W319" s="10" t="s">
         <v>380</v>
       </c>
-      <c r="X319" s="1">
+      <c r="X319" s="10">
         <v>5</v>
       </c>
     </row>
     <row r="320" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V320" s="1" t="s">
+      <c r="V320" s="10" t="s">
         <v>377</v>
       </c>
-      <c r="W320" s="1" t="s">
+      <c r="W320" s="10" t="s">
         <v>381</v>
       </c>
-      <c r="X320" s="1">
+      <c r="X320" s="10">
         <v>2</v>
       </c>
     </row>
     <row r="321" spans="22:24" x14ac:dyDescent="0.2">
-      <c r="V321" s="1" t="s">
+      <c r="V321" s="10" t="s">
         <v>377</v>
       </c>
-      <c r="W321" s="1" t="s">
+      <c r="W321" s="10" t="s">
         <v>382</v>
       </c>
-      <c r="X321" s="1">
+      <c r="X321" s="10">
         <v>32</v>
       </c>
     </row>
@@ -13327,7 +13326,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScale="116" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A12" zoomScale="116" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="Y34" sqref="Y34"/>
     </sheetView>
   </sheetViews>

</xml_diff>